<commit_message>
Updated with LLP Feedbacks
</commit_message>
<xml_diff>
--- a/Config Files/FORM-11_nodes_config.xlsx
+++ b/Config Files/FORM-11_nodes_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCA Portal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7DFA28-E817-4C1B-AAC0-27D66696BB24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C206801E-9975-48E1-B170-728B206E104B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="109">
   <si>
     <t>Field_Name</t>
   </si>
@@ -2114,10 +2114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2792,32 +2792,34 @@
       <c r="I32" s="22"/>
     </row>
     <row r="33" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="33" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="F33" s="48"/>
+      <c r="A33" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="40"/>
+      <c r="C33" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" s="43"/>
       <c r="G33" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="H33" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="I33" s="22"/>
+      <c r="H33" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="I33" s="45"/>
     </row>
     <row r="34" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34" s="60" t="s">
-        <v>78</v>
+        <v>66</v>
+      </c>
+      <c r="B34" s="33" t="s">
+        <v>77</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="9"/>
@@ -2829,205 +2831,205 @@
         <v>73</v>
       </c>
       <c r="H34" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="I34" s="22"/>
+    </row>
+    <row r="35" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="I34" s="22"/>
-    </row>
-    <row r="35" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="50"/>
+      <c r="B35" s="60" t="s">
+        <v>78</v>
+      </c>
       <c r="C35" s="13"/>
-      <c r="D35" s="61" t="s">
-        <v>74</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>47</v>
+      <c r="D35" s="9"/>
+      <c r="E35" s="35" t="s">
+        <v>45</v>
       </c>
       <c r="F35" s="48"/>
       <c r="G35" s="11" t="s">
         <v>73</v>
       </c>
       <c r="H35" s="33" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I35" s="22"/>
     </row>
     <row r="36" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="33" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B36" s="50"/>
       <c r="C36" s="13"/>
-      <c r="D36" s="16" t="s">
+      <c r="D36" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="E36" s="16" t="s">
-        <v>70</v>
+      <c r="E36" s="17" t="s">
+        <v>47</v>
       </c>
       <c r="F36" s="48"/>
       <c r="G36" s="11" t="s">
         <v>73</v>
       </c>
       <c r="H36" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="I36" s="22"/>
+    </row>
+    <row r="37" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="I36" s="22"/>
-    </row>
-    <row r="37" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="B37" s="63"/>
+      <c r="B37" s="50"/>
       <c r="C37" s="13"/>
       <c r="D37" s="16" t="s">
         <v>74</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F37" s="48"/>
-      <c r="G37" s="64" t="s">
+      <c r="G37" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="H37" s="62" t="s">
+      <c r="H37" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="I37" s="22"/>
+    </row>
+    <row r="38" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="I37" s="22"/>
-    </row>
-    <row r="38" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="65" t="s">
-        <v>79</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38" s="9"/>
+      <c r="B38" s="63"/>
+      <c r="C38" s="13"/>
       <c r="D38" s="16" t="s">
         <v>74</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="F38" s="48"/>
-      <c r="G38" s="66" t="s">
+      <c r="G38" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="H38" s="67" t="s">
+      <c r="H38" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="I38" s="22"/>
+    </row>
+    <row r="39" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="65" t="s">
         <v>79</v>
-      </c>
-      <c r="I38" s="13"/>
-    </row>
-    <row r="39" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="68" t="s">
-        <v>81</v>
       </c>
       <c r="B39" s="15" t="s">
         <v>80</v>
       </c>
       <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="35" t="s">
-        <v>45</v>
+      <c r="D39" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>39</v>
       </c>
       <c r="F39" s="48"/>
-      <c r="G39" s="11" t="s">
+      <c r="G39" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="H39" s="69" t="s">
+      <c r="H39" s="67" t="s">
+        <v>79</v>
+      </c>
+      <c r="I39" s="13"/>
+    </row>
+    <row r="40" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="68" t="s">
         <v>81</v>
-      </c>
-      <c r="I39" s="13"/>
-    </row>
-    <row r="40" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="70" t="s">
-        <v>82</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>80</v>
       </c>
       <c r="C40" s="9"/>
-      <c r="D40" s="61" t="s">
+      <c r="D40" s="9"/>
+      <c r="E40" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="F40" s="48"/>
+      <c r="G40" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H40" s="69" t="s">
+        <v>81</v>
+      </c>
+      <c r="I40" s="13"/>
+    </row>
+    <row r="41" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="70" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="E40" s="17" t="s">
+      <c r="E41" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="F40" s="71" t="s">
+      <c r="F41" s="71" t="s">
         <v>84</v>
       </c>
-      <c r="G40" s="64" t="s">
+      <c r="G41" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="H40" s="72" t="s">
+      <c r="H41" s="72" t="s">
         <v>82</v>
       </c>
-      <c r="I40" s="13"/>
-    </row>
-    <row r="41" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="73" t="s">
+      <c r="I41" s="13"/>
+    </row>
+    <row r="42" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="B41" s="74"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="38"/>
-      <c r="I41" s="14"/>
-    </row>
-    <row r="42" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="33" t="s">
+      <c r="B42" s="74"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="14"/>
+    </row>
+    <row r="43" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="50"/>
-      <c r="C42" s="15" t="s">
+      <c r="B43" s="50"/>
+      <c r="C43" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D43" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E42" s="16" t="s">
+      <c r="E43" s="16" t="s">
         <v>60</v>
-      </c>
-      <c r="F42" s="48"/>
-      <c r="G42" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="H42" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="I42" s="22"/>
-    </row>
-    <row r="43" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="B43" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="35" t="s">
-        <v>45</v>
       </c>
       <c r="F43" s="48"/>
       <c r="G43" s="11" t="s">
         <v>85</v>
       </c>
       <c r="H43" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="I43" s="22"/>
+    </row>
+    <row r="44" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="I43" s="22"/>
-    </row>
-    <row r="44" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="33" t="s">
-        <v>88</v>
-      </c>
       <c r="B44" s="33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C44" s="13"/>
       <c r="D44" s="9"/>
@@ -3039,16 +3041,16 @@
         <v>85</v>
       </c>
       <c r="H44" s="33" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I44" s="22"/>
     </row>
     <row r="45" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B45" s="33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C45" s="13"/>
       <c r="D45" s="9"/>
@@ -3060,16 +3062,16 @@
         <v>85</v>
       </c>
       <c r="H45" s="33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I45" s="22"/>
     </row>
     <row r="46" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="33" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B46" s="33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C46" s="13"/>
       <c r="D46" s="9"/>
@@ -3081,16 +3083,16 @@
         <v>85</v>
       </c>
       <c r="H46" s="33" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I46" s="22"/>
     </row>
     <row r="47" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B47" s="33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C47" s="13"/>
       <c r="D47" s="9"/>
@@ -3102,95 +3104,116 @@
         <v>85</v>
       </c>
       <c r="H47" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="I47" s="22"/>
+    </row>
+    <row r="48" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="I47" s="22"/>
-    </row>
-    <row r="48" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B48" s="50"/>
+      <c r="B48" s="33" t="s">
+        <v>95</v>
+      </c>
       <c r="C48" s="13"/>
       <c r="D48" s="9"/>
       <c r="E48" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F48" s="38"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="25"/>
-      <c r="I48" s="14"/>
-    </row>
-    <row r="49" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="33" t="s">
-        <v>97</v>
+      <c r="F48" s="48"/>
+      <c r="G48" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H48" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="I48" s="22"/>
+    </row>
+    <row r="49" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="B49" s="50"/>
-      <c r="C49" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49" s="75" t="s">
-        <v>60</v>
-      </c>
-      <c r="F49" s="11"/>
-      <c r="G49" s="60" t="s">
-        <v>96</v>
-      </c>
-      <c r="H49" s="76" t="s">
-        <v>97</v>
-      </c>
-      <c r="I49" s="22"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="F49" s="38"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="14"/>
     </row>
     <row r="50" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="B50" s="34"/>
+        <v>97</v>
+      </c>
+      <c r="B50" s="50"/>
       <c r="C50" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D50" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E50" s="77" t="s">
-        <v>99</v>
-      </c>
-      <c r="F50" s="78" t="s">
-        <v>100</v>
-      </c>
+      <c r="E50" s="75" t="s">
+        <v>60</v>
+      </c>
+      <c r="F50" s="11"/>
       <c r="G50" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="H50" s="33" t="s">
-        <v>101</v>
+      <c r="H50" s="76" t="s">
+        <v>97</v>
       </c>
       <c r="I50" s="22"/>
     </row>
     <row r="51" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="33" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B51" s="34"/>
-      <c r="C51" s="79" t="s">
+      <c r="C51" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D51" s="80" t="s">
+      <c r="D51" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E51" s="81" t="s">
-        <v>102</v>
-      </c>
-      <c r="F51" s="82"/>
+      <c r="E51" s="77" t="s">
+        <v>99</v>
+      </c>
+      <c r="F51" s="78" t="s">
+        <v>100</v>
+      </c>
       <c r="G51" s="60" t="s">
         <v>96</v>
       </c>
       <c r="H51" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="I51" s="22"/>
+    </row>
+    <row r="52" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" s="34"/>
+      <c r="C52" s="79" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="80" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="81" t="s">
+        <v>102</v>
+      </c>
+      <c r="F52" s="82"/>
+      <c r="G52" s="60" t="s">
+        <v>96</v>
+      </c>
+      <c r="H52" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="I51" s="83"/>
+      <c r="I52" s="83"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Updated with LLP Feedback Points
</commit_message>
<xml_diff>
--- a/Config Files/FORM-11_nodes_config.xlsx
+++ b/Config Files/FORM-11_nodes_config.xlsx
@@ -1,27 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCA Portal\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C206801E-9975-48E1-B170-728B206E104B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1-1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1-1" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="109">
   <si>
     <t>Field_Name</t>
   </si>
@@ -63,6 +54,286 @@
   </si>
   <si>
     <t>STREET</t>
+  </si>
+  <si>
+    <t>LLP</t>
+  </si>
+  <si>
+    <t>ba_address_line1</t>
+  </si>
+  <si>
+    <t>address_line2</t>
+  </si>
+  <si>
+    <t>HOUSE_NUMBER</t>
+  </si>
+  <si>
+    <t>ba_address_line2</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
+    <t>ba_city</t>
+  </si>
+  <si>
+    <t>pincode</t>
+  </si>
+  <si>
+    <t>POSTAL_PINCODE</t>
+  </si>
+  <si>
+    <t>ba_pincode</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>REGION_STATE</t>
+  </si>
+  <si>
+    <t>ba_state</t>
+  </si>
+  <si>
+    <t>last_annual_returns_filed_date</t>
+  </si>
+  <si>
+    <t>ZMCA_LLP_FORM12</t>
+  </si>
+  <si>
+    <t>STRT_DATE_FIN_YR</t>
+  </si>
+  <si>
+    <t>last_filing_date</t>
+  </si>
+  <si>
+    <t>directors</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>T_FORM11_SECTN10/DATA</t>
+  </si>
+  <si>
+    <t>SIGNER_ID,SIGNER_ID,DESIGNATION,NATIONALITY</t>
+  </si>
+  <si>
+    <t>authorized_signatories</t>
+  </si>
+  <si>
+    <t>din,pan,designation,nationality</t>
+  </si>
+  <si>
+    <t>din</t>
+  </si>
+  <si>
+    <t>SIGNER_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if SIGNER_ID is only number </t>
+  </si>
+  <si>
+    <t>pan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if SIGNER_ID is aplhanumeric </t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>NOT ABLE TO GET FROM XML</t>
+  </si>
+  <si>
+    <t>designation</t>
+  </si>
+  <si>
+    <t>DESIGNATION</t>
+  </si>
+  <si>
+    <t>date_of_appointment</t>
+  </si>
+  <si>
+    <t>Date of Appointment</t>
+  </si>
+  <si>
+    <t>date_of_cessation</t>
+  </si>
+  <si>
+    <t>Date of Cessation</t>
+  </si>
+  <si>
+    <t>nationality</t>
+  </si>
+  <si>
+    <t>NATIONALITY</t>
+  </si>
+  <si>
+    <t>father_name</t>
+  </si>
+  <si>
+    <t>Fathers name</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>Permanent Residential Address</t>
+  </si>
+  <si>
+    <t>contribution_details</t>
+  </si>
+  <si>
+    <t>financial_year</t>
+  </si>
+  <si>
+    <t>ANNUAL_RETURN</t>
+  </si>
+  <si>
+    <t>individual_partners</t>
+  </si>
+  <si>
+    <t>SIGNER_ID,id_type,DESIGNATION,OBL_CONTRI,CONTRI_REC</t>
+  </si>
+  <si>
+    <t>signer_id,id_type,designation,obligation_contribution,received_contribution</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>signer_id</t>
+  </si>
+  <si>
+    <t>id_type</t>
+  </si>
+  <si>
+    <t>LOGIC</t>
+  </si>
+  <si>
+    <t>IF APLHANUMERIC PAN.ONLY NUMBERS MEANS DIN</t>
+  </si>
+  <si>
+    <t>obligation_contribution</t>
+  </si>
+  <si>
+    <t>OBL_CONTRI</t>
+  </si>
+  <si>
+    <t>received_contribution</t>
+  </si>
+  <si>
+    <t>CONTRI_REC</t>
+  </si>
+  <si>
+    <t>body_corporates</t>
+  </si>
+  <si>
+    <t>T_FORM11_SECTN11/DATA</t>
+  </si>
+  <si>
+    <t>DESIGNATION,OBL_CONTRI,CONTRI_REC,SIGNER_ID,nominee_id_type</t>
+  </si>
+  <si>
+    <t>designation,obligation_contribution,received_contribution,nominee_id,nominee_id_type</t>
+  </si>
+  <si>
+    <t>CIN / LLP corporate type</t>
+  </si>
+  <si>
+    <t>Name of the body corporate</t>
+  </si>
+  <si>
+    <t>nominee_id</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>nominee_name</t>
+  </si>
+  <si>
+    <t>nominee_id_type</t>
+  </si>
+  <si>
+    <t>DIN/PAN/PASSPORT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  as per nominee_id we get from Form 11
+DIN-7 digit/
+PAN-10digit alpha numeric/
+Passport-others</t>
+  </si>
+  <si>
+    <t>summary_designated_partners</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>Category " type of category like Individuals, LLPs , company etc" and multipe for each Category
+Logic - Based on Each type, we need to create below sub fields &amp; capture the details in respective column</t>
+  </si>
+  <si>
+    <t>partner</t>
+  </si>
+  <si>
+    <t>Number of Partners</t>
+  </si>
+  <si>
+    <t>indian_desig_partner</t>
+  </si>
+  <si>
+    <t>Resident in India</t>
+  </si>
+  <si>
+    <t>other_desig_partner</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>principal_business_activities</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>business_classification</t>
+  </si>
+  <si>
+    <t>BUSINESS_CLASS</t>
+  </si>
+  <si>
+    <t>(half name is coming in xml)</t>
+  </si>
+  <si>
+    <t>main_activity_group_description</t>
+  </si>
+  <si>
+    <t>PRIN_ACTIVITY</t>
+  </si>
+  <si>
+    <t>business_activity_description</t>
+  </si>
+  <si>
+    <t>Multiple</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
   <si>
     <r>
@@ -75,299 +346,32 @@
     </r>
   </si>
   <si>
-    <t>ba_address_line1</t>
-  </si>
-  <si>
-    <t>address_line2</t>
-  </si>
-  <si>
-    <t>HOUSE_NUMBER</t>
-  </si>
-  <si>
-    <t>ba_address_line2</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>CITY</t>
-  </si>
-  <si>
-    <t>ba_city</t>
-  </si>
-  <si>
-    <t>pincode</t>
-  </si>
-  <si>
-    <t>POSTAL_PINCODE</t>
-  </si>
-  <si>
-    <t>ba_pincode</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>REGION_STATE</t>
-  </si>
-  <si>
-    <t>ba_state</t>
-  </si>
-  <si>
-    <t>last_annual_returns_filed_date</t>
-  </si>
-  <si>
-    <t>ZMCA_LLP_FORM12</t>
-  </si>
-  <si>
-    <t>STRT_DATE_FIN_YR</t>
-  </si>
-  <si>
-    <t>last_filing_date</t>
-  </si>
-  <si>
-    <t>directors</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>T_FORM11_SECTN10/DATA</t>
-  </si>
-  <si>
-    <t>SIGNER_ID,SIGNER_ID,DESIGNATION,NATIONALITY</t>
-  </si>
-  <si>
-    <t>authorized_signatories</t>
-  </si>
-  <si>
-    <t>din,pan,designation,nationality</t>
-  </si>
-  <si>
-    <t>din</t>
-  </si>
-  <si>
-    <t>SIGNER_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if SIGNER_ID is only number </t>
-  </si>
-  <si>
-    <t>pan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if SIGNER_ID is aplhanumeric </t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>NOT ABLE TO GET FROM XML</t>
-  </si>
-  <si>
-    <t>designation</t>
-  </si>
-  <si>
-    <t>DESIGNATION</t>
-  </si>
-  <si>
-    <t>date_of_appointment</t>
-  </si>
-  <si>
-    <t>Date of Appointment</t>
-  </si>
-  <si>
-    <t>date_of_cessation</t>
-  </si>
-  <si>
-    <t>Date of Cessation</t>
-  </si>
-  <si>
-    <t>nationality</t>
-  </si>
-  <si>
-    <t>NATIONALITY</t>
-  </si>
-  <si>
-    <t>father_name</t>
-  </si>
-  <si>
-    <t>Fathers name</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>Permanent Residential Address</t>
-  </si>
-  <si>
-    <t>contribution_details</t>
-  </si>
-  <si>
-    <t>financial_year</t>
-  </si>
-  <si>
-    <t>ANNUAL_RETURN</t>
-  </si>
-  <si>
-    <t>individual_partners</t>
-  </si>
-  <si>
-    <t>SIGNER_ID,id_type,DESIGNATION,OBL_CONTRI,CONTRI_REC</t>
-  </si>
-  <si>
-    <t>signer_id,id_type,designation,obligation_contribution,received_contribution</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>signer_id</t>
-  </si>
-  <si>
-    <t>id_type</t>
-  </si>
-  <si>
-    <t>LOGIC</t>
-  </si>
-  <si>
-    <t>IF APLHANUMERIC PAN.ONLY NUMBERS MEANS DIN</t>
-  </si>
-  <si>
-    <t>obligation_contribution</t>
-  </si>
-  <si>
-    <t>OBL_CONTRI</t>
-  </si>
-  <si>
-    <t>received_contribution</t>
-  </si>
-  <si>
-    <t>CONTRI_REC</t>
-  </si>
-  <si>
-    <t>body_corporates</t>
-  </si>
-  <si>
-    <t>T_FORM11_SECTN11/DATA</t>
-  </si>
-  <si>
-    <t>DESIGNATION,OBL_CONTRI,CONTRI_REC,SIGNER_ID,nominee_id_type</t>
-  </si>
-  <si>
-    <t>designation,obligation_contribution,received_contribution,nominee_id,nominee_id_type</t>
-  </si>
-  <si>
-    <t>CIN / LLP corporate type</t>
-  </si>
-  <si>
-    <t>Name of the body corporate</t>
-  </si>
-  <si>
-    <t>nominee_id</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>nominee_name</t>
-  </si>
-  <si>
-    <t>nominee_id_type</t>
-  </si>
-  <si>
-    <t>DIN/PAN/PASSPORT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  as per nominee_id we get from Form 11
-DIN-7 digit/
-PAN-10digit alpha numeric/
-Passport-others</t>
-  </si>
-  <si>
-    <t>summary_designated_partners</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>Category " type of category like Individuals, LLPs , company etc" and multipe for each Category
-Logic - Based on Each type, we need to create below sub fields &amp; capture the details in respective column</t>
-  </si>
-  <si>
-    <t>partner</t>
-  </si>
-  <si>
-    <t>Number of Partners</t>
-  </si>
-  <si>
-    <t>indian_desig_partner</t>
-  </si>
-  <si>
-    <t>Resident in India</t>
-  </si>
-  <si>
-    <t>other_desig_partner</t>
-  </si>
-  <si>
-    <t>Others</t>
-  </si>
-  <si>
-    <t>total</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>principal_business_activities</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>business_classification</t>
-  </si>
-  <si>
-    <t>BUSINESS_CLASS</t>
-  </si>
-  <si>
-    <t>(half name is coming in xml)</t>
-  </si>
-  <si>
-    <t>main_activity_group_description</t>
-  </si>
-  <si>
-    <t>PRIN_ACTIVITY</t>
-  </si>
-  <si>
-    <t>business_activity_description</t>
-  </si>
-  <si>
-    <t>Multiple</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>T_FORM11_SECTN10 dd:minOccur="0"/DATA dd:maxOccur="-1"</t>
   </si>
   <si>
     <t>BUSINESS_CLASS(hlf name is coming in xml)</t>
-  </si>
-  <si>
-    <t>LLP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="0" formatCode="General"/>
+  </numFmts>
+  <fonts count="13">
     <font>
       <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -387,19 +391,19 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="10"/>
       <color indexed="15"/>
       <name val="Courier New"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="10"/>
       <color indexed="19"/>
       <name val="Courier New"/>
@@ -420,7 +424,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="10"/>
       <color indexed="20"/>
       <name val="Courier New"/>
@@ -831,159 +835,290 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="92">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="93">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -992,85 +1127,36 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFD8D8D8"/>
-      <rgbColor rgb="FFA5A5A5"/>
-      <rgbColor rgb="FFAAAAAA"/>
-      <rgbColor rgb="FF92D050"/>
-      <rgbColor rgb="FF1D1D1C"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FF881280"/>
-      <rgbColor rgb="FF444444"/>
-      <rgbColor rgb="FFA5A5A5"/>
-      <rgbColor rgb="FFF8FF61"/>
-      <rgbColor rgb="FF7030A0"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FFFCFF40"/>
-      <rgbColor rgb="FFF9FF5A"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffd8d8d8"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff92d050"/>
+      <rgbColor rgb="ff1d1d1c"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ff881280"/>
+      <rgbColor rgb="ff444444"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="fff8ff61"/>
+      <rgbColor rgb="ff7030a0"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="fffcff40"/>
+      <rgbColor rgb="fff9ff5a"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -1272,7 +1358,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1290,7 +1376,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1319,7 +1405,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1344,7 +1430,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1369,7 +1455,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1394,7 +1480,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1419,7 +1505,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1444,7 +1530,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1469,7 +1555,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1494,7 +1580,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1519,7 +1605,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1532,15 +1618,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1557,7 +1637,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1575,7 +1655,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1600,7 +1680,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1625,7 +1705,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1650,7 +1730,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1675,7 +1755,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1700,7 +1780,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1725,7 +1805,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1750,7 +1830,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1775,7 +1855,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1800,7 +1880,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1813,15 +1893,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1835,7 +1909,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1853,7 +1927,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1882,7 +1956,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1907,7 +1981,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1932,7 +2006,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1957,7 +2031,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1982,7 +2056,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2007,7 +2081,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2032,7 +2106,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2057,7 +2131,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2082,7 +2156,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2095,75 +2169,65 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I52"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="38.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="42.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="38.1719" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.3516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.3516" style="1" customWidth="1"/>
     <col min="4" max="4" width="28" style="1" customWidth="1"/>
     <col min="5" max="5" width="33" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="1"/>
+    <col min="6" max="6" width="26.3516" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.1719" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6719" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="13.55" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
       <c r="F1" s="4"/>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" t="s" s="5">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" ht="13.55" customHeight="1">
+      <c r="A2" t="s" s="6">
         <v>8</v>
       </c>
       <c r="B2" s="7"/>
@@ -2175,8 +2239,8 @@
       <c r="H2" s="8"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="s" s="11">
         <v>9</v>
       </c>
       <c r="B3" s="12"/>
@@ -2188,146 +2252,146 @@
       <c r="H3" s="9"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="s" s="11">
         <v>10</v>
       </c>
       <c r="B4" s="12"/>
-      <c r="C4" s="15" t="s">
+      <c r="C4" t="s" s="15">
         <v>11</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" t="s" s="16">
         <v>13</v>
       </c>
       <c r="F4" s="9"/>
-      <c r="G4" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="H4" s="18" t="s">
+      <c r="G4" t="s" s="17">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s" s="18">
         <v>15</v>
       </c>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" t="s" s="11">
         <v>16</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="15" t="s">
+      <c r="C5" t="s" s="15">
         <v>11</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" t="s" s="17">
         <v>17</v>
       </c>
       <c r="F5" s="9"/>
-      <c r="G5" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="H5" s="18" t="s">
+      <c r="G5" t="s" s="17">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s" s="18">
         <v>18</v>
       </c>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" t="s" s="11">
         <v>19</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="15" t="s">
+      <c r="C6" t="s" s="15">
         <v>11</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" t="s" s="16">
         <v>20</v>
       </c>
       <c r="F6" s="9"/>
-      <c r="G6" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="H6" s="18" t="s">
+      <c r="G6" t="s" s="17">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s" s="18">
         <v>21</v>
       </c>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" t="s" s="11">
         <v>22</v>
       </c>
       <c r="B7" s="12"/>
-      <c r="C7" s="15" t="s">
+      <c r="C7" t="s" s="15">
         <v>11</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" t="s" s="17">
         <v>23</v>
       </c>
       <c r="F7" s="9"/>
-      <c r="G7" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="H7" s="18" t="s">
+      <c r="G7" t="s" s="17">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s" s="18">
         <v>24</v>
       </c>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" t="s" s="11">
         <v>25</v>
       </c>
       <c r="B8" s="12"/>
-      <c r="C8" s="15" t="s">
+      <c r="C8" t="s" s="15">
         <v>11</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" t="s" s="16">
         <v>26</v>
       </c>
       <c r="F8" s="9"/>
-      <c r="G8" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="H8" s="19" t="s">
+      <c r="G8" t="s" s="17">
+        <v>14</v>
+      </c>
+      <c r="H8" t="s" s="19">
         <v>27</v>
       </c>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+    <row r="9" ht="14" customHeight="1">
+      <c r="A9" t="s" s="11">
         <v>28</v>
       </c>
       <c r="B9" s="20"/>
-      <c r="C9" s="15" t="s">
+      <c r="C9" t="s" s="15">
         <v>11</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" t="s" s="16">
         <v>29</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" t="s" s="16">
         <v>30</v>
       </c>
       <c r="F9" s="9"/>
-      <c r="G9" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="H9" s="11" t="s">
+      <c r="G9" t="s" s="21">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s" s="11">
         <v>31</v>
       </c>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" t="s" s="23">
         <v>32</v>
       </c>
       <c r="B10" s="24"/>
@@ -2339,222 +2403,222 @@
       <c r="H10" s="25"/>
       <c r="I10" s="14"/>
     </row>
-    <row r="11" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+    <row r="11" ht="14" customHeight="1">
+      <c r="A11" t="s" s="26">
         <v>32</v>
       </c>
       <c r="B11" s="27"/>
-      <c r="C11" s="28" t="s">
+      <c r="C11" t="s" s="28">
         <v>33</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" t="s" s="29">
         <v>34</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" t="s" s="29">
         <v>35</v>
       </c>
       <c r="F11" s="30"/>
-      <c r="G11" s="31" t="s">
+      <c r="G11" t="s" s="31">
         <v>36</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="H11" t="s" s="26">
         <v>37</v>
       </c>
       <c r="I11" s="32"/>
     </row>
-    <row r="12" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+    <row r="12" ht="14" customHeight="1">
+      <c r="A12" t="s" s="33">
         <v>38</v>
       </c>
       <c r="B12" s="34"/>
       <c r="C12" s="13"/>
-      <c r="D12" s="16" t="s">
+      <c r="D12" t="s" s="16">
         <v>34</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" t="s" s="16">
         <v>39</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" t="s" s="17">
         <v>40</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="G12" t="s" s="21">
         <v>36</v>
       </c>
-      <c r="H12" s="33" t="s">
+      <c r="H12" t="s" s="33">
         <v>38</v>
       </c>
       <c r="I12" s="22"/>
     </row>
-    <row r="13" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+    <row r="13" ht="14" customHeight="1">
+      <c r="A13" t="s" s="33">
         <v>41</v>
       </c>
       <c r="B13" s="34"/>
       <c r="C13" s="13"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="16" t="s">
+      <c r="E13" t="s" s="16">
         <v>39</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" t="s" s="17">
         <v>42</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" t="s" s="21">
         <v>36</v>
       </c>
-      <c r="H13" s="33" t="s">
+      <c r="H13" t="s" s="33">
         <v>41</v>
       </c>
       <c r="I13" s="22"/>
     </row>
-    <row r="14" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+    <row r="14" ht="14" customHeight="1">
+      <c r="A14" t="s" s="33">
         <v>43</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" t="s" s="33">
         <v>44</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="35" t="s">
+      <c r="E14" t="s" s="35">
         <v>45</v>
       </c>
       <c r="F14" s="9"/>
-      <c r="G14" s="21" t="s">
+      <c r="G14" t="s" s="21">
         <v>36</v>
       </c>
-      <c r="H14" s="33" t="s">
+      <c r="H14" t="s" s="33">
         <v>43</v>
       </c>
       <c r="I14" s="22"/>
     </row>
-    <row r="15" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+    <row r="15" ht="14" customHeight="1">
+      <c r="A15" t="s" s="33">
         <v>46</v>
       </c>
       <c r="B15" s="34"/>
       <c r="C15" s="13"/>
-      <c r="D15" s="16" t="s">
+      <c r="D15" t="s" s="16">
         <v>34</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" t="s" s="16">
         <v>47</v>
       </c>
       <c r="F15" s="9"/>
-      <c r="G15" s="21" t="s">
+      <c r="G15" t="s" s="21">
         <v>36</v>
       </c>
-      <c r="H15" s="33" t="s">
+      <c r="H15" t="s" s="33">
         <v>46</v>
       </c>
       <c r="I15" s="22"/>
     </row>
-    <row r="16" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+    <row r="16" ht="14" customHeight="1">
+      <c r="A16" t="s" s="33">
         <v>48</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" t="s" s="33">
         <v>49</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="35" t="s">
+      <c r="E16" t="s" s="35">
         <v>45</v>
       </c>
       <c r="F16" s="9"/>
-      <c r="G16" s="21" t="s">
+      <c r="G16" t="s" s="21">
         <v>36</v>
       </c>
-      <c r="H16" s="33" t="s">
+      <c r="H16" t="s" s="33">
         <v>48</v>
       </c>
       <c r="I16" s="22"/>
     </row>
-    <row r="17" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+    <row r="17" ht="14" customHeight="1">
+      <c r="A17" t="s" s="33">
         <v>50</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" t="s" s="11">
         <v>51</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="35" t="s">
+      <c r="E17" t="s" s="35">
         <v>45</v>
       </c>
       <c r="F17" s="9"/>
-      <c r="G17" s="21" t="s">
+      <c r="G17" t="s" s="21">
         <v>36</v>
       </c>
-      <c r="H17" s="33" t="s">
+      <c r="H17" t="s" s="33">
         <v>50</v>
       </c>
       <c r="I17" s="22"/>
     </row>
-    <row r="18" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
+    <row r="18" ht="14" customHeight="1">
+      <c r="A18" t="s" s="33">
         <v>52</v>
       </c>
       <c r="B18" s="34"/>
       <c r="C18" s="13"/>
-      <c r="D18" s="16" t="s">
+      <c r="D18" t="s" s="16">
         <v>34</v>
       </c>
-      <c r="E18" s="36" t="s">
+      <c r="E18" t="s" s="36">
         <v>53</v>
       </c>
       <c r="F18" s="9"/>
-      <c r="G18" s="21" t="s">
+      <c r="G18" t="s" s="21">
         <v>36</v>
       </c>
-      <c r="H18" s="33" t="s">
+      <c r="H18" t="s" s="33">
         <v>52</v>
       </c>
       <c r="I18" s="22"/>
     </row>
-    <row r="19" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+    <row r="19" ht="14" customHeight="1">
+      <c r="A19" t="s" s="33">
         <v>54</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" t="s" s="33">
         <v>55</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="9"/>
-      <c r="E19" s="35" t="s">
+      <c r="E19" t="s" s="35">
         <v>45</v>
       </c>
       <c r="F19" s="9"/>
-      <c r="G19" s="21" t="s">
+      <c r="G19" t="s" s="21">
         <v>36</v>
       </c>
-      <c r="H19" s="33" t="s">
+      <c r="H19" t="s" s="33">
         <v>54</v>
       </c>
       <c r="I19" s="22"/>
     </row>
-    <row r="20" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
+    <row r="20" ht="14" customHeight="1">
+      <c r="A20" t="s" s="33">
         <v>56</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" t="s" s="33">
         <v>57</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="35" t="s">
+      <c r="E20" t="s" s="35">
         <v>45</v>
       </c>
       <c r="F20" s="9"/>
-      <c r="G20" s="21" t="s">
+      <c r="G20" t="s" s="21">
         <v>36</v>
       </c>
-      <c r="H20" s="33" t="s">
+      <c r="H20" t="s" s="33">
         <v>56</v>
       </c>
       <c r="I20" s="22"/>
     </row>
-    <row r="21" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
+    <row r="21" ht="13.55" customHeight="1">
+      <c r="A21" t="s" s="37">
         <v>58</v>
       </c>
       <c r="B21" s="24"/>
@@ -2566,179 +2630,179 @@
       <c r="H21" s="25"/>
       <c r="I21" s="14"/>
     </row>
-    <row r="22" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+    <row r="22" ht="14" customHeight="1">
+      <c r="A22" t="s" s="39">
         <v>59</v>
       </c>
       <c r="B22" s="40"/>
-      <c r="C22" s="41" t="s">
+      <c r="C22" t="s" s="41">
         <v>11</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D22" t="s" s="42">
         <v>12</v>
       </c>
-      <c r="E22" s="42" t="s">
+      <c r="E22" t="s" s="42">
         <v>60</v>
       </c>
       <c r="F22" s="43"/>
-      <c r="G22" s="44" t="s">
+      <c r="G22" t="s" s="44">
         <v>61</v>
       </c>
-      <c r="H22" s="39" t="s">
+      <c r="H22" t="s" s="39">
         <v>59</v>
       </c>
       <c r="I22" s="45"/>
     </row>
-    <row r="23" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="44" t="s">
+    <row r="23" ht="14" customHeight="1">
+      <c r="A23" t="s" s="44">
         <v>61</v>
       </c>
       <c r="B23" s="40"/>
-      <c r="C23" s="41" t="s">
+      <c r="C23" t="s" s="41">
         <v>33</v>
       </c>
-      <c r="D23" s="42" t="s">
+      <c r="D23" t="s" s="42">
         <v>34</v>
       </c>
-      <c r="E23" s="42" t="s">
+      <c r="E23" t="s" s="42">
         <v>62</v>
       </c>
       <c r="F23" s="43"/>
-      <c r="G23" s="44" t="s">
+      <c r="G23" t="s" s="44">
         <v>61</v>
       </c>
-      <c r="H23" s="46" t="s">
+      <c r="H23" t="s" s="46">
         <v>63</v>
       </c>
       <c r="I23" s="47"/>
     </row>
-    <row r="24" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="33" t="s">
+    <row r="24" ht="14" customHeight="1">
+      <c r="A24" t="s" s="33">
         <v>64</v>
       </c>
       <c r="B24" s="34"/>
       <c r="C24" s="13"/>
       <c r="D24" s="9"/>
-      <c r="E24" s="16" t="s">
+      <c r="E24" t="s" s="16">
         <v>39</v>
       </c>
       <c r="F24" s="48"/>
-      <c r="G24" s="11" t="s">
+      <c r="G24" t="s" s="11">
         <v>61</v>
       </c>
-      <c r="H24" s="33" t="s">
+      <c r="H24" t="s" s="33">
         <v>65</v>
       </c>
       <c r="I24" s="22"/>
     </row>
-    <row r="25" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+    <row r="25" ht="30.75" customHeight="1">
+      <c r="A25" t="s" s="33">
         <v>66</v>
       </c>
       <c r="B25" s="34"/>
       <c r="C25" s="13"/>
-      <c r="D25" s="17" t="s">
+      <c r="D25" t="s" s="17">
         <v>67</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" t="s" s="16">
         <v>66</v>
       </c>
-      <c r="F25" s="49" t="s">
+      <c r="F25" t="s" s="49">
         <v>68</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G25" t="s" s="11">
         <v>61</v>
       </c>
-      <c r="H25" s="33" t="s">
+      <c r="H25" t="s" s="33">
         <v>66</v>
       </c>
       <c r="I25" s="22"/>
     </row>
-    <row r="26" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="33" t="s">
+    <row r="26" ht="14" customHeight="1">
+      <c r="A26" t="s" s="33">
         <v>43</v>
       </c>
-      <c r="B26" s="33" t="s">
+      <c r="B26" t="s" s="33">
         <v>44</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="9"/>
-      <c r="E26" s="35" t="s">
+      <c r="E26" t="s" s="35">
         <v>45</v>
       </c>
       <c r="F26" s="48"/>
-      <c r="G26" s="11" t="s">
+      <c r="G26" t="s" s="11">
         <v>61</v>
       </c>
-      <c r="H26" s="33" t="s">
+      <c r="H26" t="s" s="33">
         <v>43</v>
       </c>
       <c r="I26" s="22"/>
     </row>
-    <row r="27" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
+    <row r="27" ht="14" customHeight="1">
+      <c r="A27" t="s" s="33">
         <v>46</v>
       </c>
       <c r="B27" s="34"/>
       <c r="C27" s="13"/>
-      <c r="D27" s="16" t="s">
+      <c r="D27" t="s" s="16">
         <v>34</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" t="s" s="16">
         <v>47</v>
       </c>
       <c r="F27" s="48"/>
-      <c r="G27" s="11" t="s">
+      <c r="G27" t="s" s="11">
         <v>61</v>
       </c>
-      <c r="H27" s="33" t="s">
+      <c r="H27" t="s" s="33">
         <v>46</v>
       </c>
       <c r="I27" s="22"/>
     </row>
-    <row r="28" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="33" t="s">
+    <row r="28" ht="14" customHeight="1">
+      <c r="A28" t="s" s="33">
         <v>69</v>
       </c>
       <c r="B28" s="34"/>
       <c r="C28" s="13"/>
-      <c r="D28" s="16" t="s">
+      <c r="D28" t="s" s="16">
         <v>34</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" t="s" s="16">
         <v>70</v>
       </c>
       <c r="F28" s="48"/>
-      <c r="G28" s="11" t="s">
+      <c r="G28" t="s" s="11">
         <v>61</v>
       </c>
-      <c r="H28" s="33" t="s">
+      <c r="H28" t="s" s="33">
         <v>69</v>
       </c>
       <c r="I28" s="22"/>
     </row>
-    <row r="29" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="33" t="s">
+    <row r="29" ht="14" customHeight="1">
+      <c r="A29" t="s" s="33">
         <v>71</v>
       </c>
       <c r="B29" s="34"/>
       <c r="C29" s="13"/>
-      <c r="D29" s="16" t="s">
+      <c r="D29" t="s" s="16">
         <v>34</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="E29" t="s" s="16">
         <v>72</v>
       </c>
       <c r="F29" s="48"/>
-      <c r="G29" s="11" t="s">
+      <c r="G29" t="s" s="11">
         <v>61</v>
       </c>
-      <c r="H29" s="33" t="s">
+      <c r="H29" t="s" s="33">
         <v>71</v>
       </c>
       <c r="I29" s="22"/>
     </row>
-    <row r="30" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" ht="13.55" customHeight="1">
       <c r="A30" s="50"/>
       <c r="B30" s="20"/>
       <c r="C30" s="13"/>
@@ -2749,479 +2813,452 @@
       <c r="H30" s="25"/>
       <c r="I30" s="14"/>
     </row>
-    <row r="31" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="51" t="s">
+    <row r="31" ht="39.55" customHeight="1">
+      <c r="A31" t="s" s="51">
         <v>73</v>
       </c>
       <c r="B31" s="52"/>
-      <c r="C31" s="53" t="s">
+      <c r="C31" t="s" s="53">
         <v>33</v>
       </c>
-      <c r="D31" s="54" t="s">
+      <c r="D31" t="s" s="54">
         <v>74</v>
       </c>
-      <c r="E31" s="55" t="s">
+      <c r="E31" t="s" s="55">
         <v>75</v>
       </c>
       <c r="F31" s="56"/>
-      <c r="G31" s="51" t="s">
+      <c r="G31" t="s" s="51">
         <v>73</v>
       </c>
-      <c r="H31" s="57" t="s">
+      <c r="H31" t="s" s="57">
         <v>76</v>
       </c>
       <c r="I31" s="58"/>
     </row>
-    <row r="32" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="s">
+    <row r="32" ht="14" customHeight="1">
+      <c r="A32" t="s" s="33">
         <v>64</v>
       </c>
       <c r="B32" s="20"/>
       <c r="C32" s="13"/>
       <c r="D32" s="59"/>
-      <c r="E32" s="35" t="s">
+      <c r="E32" t="s" s="35">
         <v>45</v>
       </c>
       <c r="F32" s="48"/>
-      <c r="G32" s="11" t="s">
+      <c r="G32" t="s" s="11">
         <v>73</v>
       </c>
-      <c r="H32" s="33" t="s">
+      <c r="H32" t="s" s="33">
         <v>65</v>
       </c>
       <c r="I32" s="22"/>
     </row>
-    <row r="33" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" s="40"/>
-      <c r="C33" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="F33" s="43"/>
-      <c r="G33" s="11" t="s">
+    <row r="33" ht="14" customHeight="1">
+      <c r="A33" t="s" s="33">
+        <v>66</v>
+      </c>
+      <c r="B33" t="s" s="33">
+        <v>77</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="9"/>
+      <c r="E33" t="s" s="35">
+        <v>45</v>
+      </c>
+      <c r="F33" s="48"/>
+      <c r="G33" t="s" s="11">
         <v>73</v>
       </c>
-      <c r="H33" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="I33" s="45"/>
-    </row>
-    <row r="34" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
+      <c r="H33" t="s" s="33">
         <v>66</v>
       </c>
-      <c r="B34" s="33" t="s">
-        <v>77</v>
+      <c r="I33" s="22"/>
+    </row>
+    <row r="34" ht="14" customHeight="1">
+      <c r="A34" t="s" s="33">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s" s="60">
+        <v>78</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="9"/>
-      <c r="E34" s="35" t="s">
+      <c r="E34" t="s" s="35">
         <v>45</v>
       </c>
       <c r="F34" s="48"/>
-      <c r="G34" s="11" t="s">
+      <c r="G34" t="s" s="11">
         <v>73</v>
       </c>
-      <c r="H34" s="33" t="s">
-        <v>66</v>
+      <c r="H34" t="s" s="33">
+        <v>43</v>
       </c>
       <c r="I34" s="22"/>
     </row>
-    <row r="35" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="60" t="s">
-        <v>78</v>
-      </c>
+    <row r="35" ht="37.5" customHeight="1">
+      <c r="A35" t="s" s="33">
+        <v>46</v>
+      </c>
+      <c r="B35" s="50"/>
       <c r="C35" s="13"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="35" t="s">
-        <v>45</v>
+      <c r="D35" t="s" s="61">
+        <v>74</v>
+      </c>
+      <c r="E35" t="s" s="17">
+        <v>47</v>
       </c>
       <c r="F35" s="48"/>
-      <c r="G35" s="11" t="s">
+      <c r="G35" t="s" s="11">
         <v>73</v>
       </c>
-      <c r="H35" s="33" t="s">
-        <v>43</v>
+      <c r="H35" t="s" s="33">
+        <v>46</v>
       </c>
       <c r="I35" s="22"/>
     </row>
-    <row r="36" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="33" t="s">
-        <v>46</v>
+    <row r="36" ht="37.5" customHeight="1">
+      <c r="A36" t="s" s="33">
+        <v>69</v>
       </c>
       <c r="B36" s="50"/>
       <c r="C36" s="13"/>
-      <c r="D36" s="61" t="s">
+      <c r="D36" t="s" s="16">
         <v>74</v>
       </c>
-      <c r="E36" s="17" t="s">
-        <v>47</v>
+      <c r="E36" t="s" s="16">
+        <v>70</v>
       </c>
       <c r="F36" s="48"/>
-      <c r="G36" s="11" t="s">
+      <c r="G36" t="s" s="11">
         <v>73</v>
       </c>
-      <c r="H36" s="33" t="s">
-        <v>46</v>
+      <c r="H36" t="s" s="33">
+        <v>69</v>
       </c>
       <c r="I36" s="22"/>
     </row>
-    <row r="37" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" s="50"/>
+    <row r="37" ht="37.5" customHeight="1">
+      <c r="A37" t="s" s="62">
+        <v>71</v>
+      </c>
+      <c r="B37" s="63"/>
       <c r="C37" s="13"/>
-      <c r="D37" s="16" t="s">
+      <c r="D37" t="s" s="16">
         <v>74</v>
       </c>
-      <c r="E37" s="16" t="s">
-        <v>70</v>
+      <c r="E37" t="s" s="16">
+        <v>72</v>
       </c>
       <c r="F37" s="48"/>
-      <c r="G37" s="11" t="s">
+      <c r="G37" t="s" s="64">
         <v>73</v>
       </c>
-      <c r="H37" s="33" t="s">
-        <v>69</v>
+      <c r="H37" t="s" s="62">
+        <v>71</v>
       </c>
       <c r="I37" s="22"/>
     </row>
-    <row r="38" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="63"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="16" t="s">
+    <row r="38" ht="37.5" customHeight="1">
+      <c r="A38" t="s" s="65">
+        <v>79</v>
+      </c>
+      <c r="B38" t="s" s="15">
+        <v>80</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" t="s" s="16">
         <v>74</v>
       </c>
-      <c r="E38" s="16" t="s">
-        <v>72</v>
+      <c r="E38" t="s" s="16">
+        <v>39</v>
       </c>
       <c r="F38" s="48"/>
-      <c r="G38" s="64" t="s">
+      <c r="G38" t="s" s="66">
         <v>73</v>
       </c>
-      <c r="H38" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I38" s="22"/>
-    </row>
-    <row r="39" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="65" t="s">
+      <c r="H38" t="s" s="67">
         <v>79</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="I38" s="13"/>
+    </row>
+    <row r="39" ht="37.5" customHeight="1">
+      <c r="A39" t="s" s="68">
+        <v>81</v>
+      </c>
+      <c r="B39" t="s" s="15">
         <v>80</v>
       </c>
       <c r="C39" s="9"/>
-      <c r="D39" s="16" t="s">
+      <c r="D39" s="9"/>
+      <c r="E39" t="s" s="35">
+        <v>45</v>
+      </c>
+      <c r="F39" s="48"/>
+      <c r="G39" t="s" s="11">
+        <v>73</v>
+      </c>
+      <c r="H39" t="s" s="69">
+        <v>81</v>
+      </c>
+      <c r="I39" s="13"/>
+    </row>
+    <row r="40" ht="37.5" customHeight="1">
+      <c r="A40" t="s" s="70">
+        <v>82</v>
+      </c>
+      <c r="B40" t="s" s="15">
+        <v>80</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" t="s" s="61">
         <v>74</v>
       </c>
-      <c r="E39" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F39" s="48"/>
-      <c r="G39" s="66" t="s">
+      <c r="E40" t="s" s="17">
+        <v>83</v>
+      </c>
+      <c r="F40" t="s" s="71">
+        <v>84</v>
+      </c>
+      <c r="G40" t="s" s="64">
         <v>73</v>
       </c>
-      <c r="H39" s="67" t="s">
-        <v>79</v>
-      </c>
-      <c r="I39" s="13"/>
-    </row>
-    <row r="40" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="68" t="s">
-        <v>81</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="35" t="s">
+      <c r="H40" t="s" s="72">
+        <v>82</v>
+      </c>
+      <c r="I40" s="13"/>
+    </row>
+    <row r="41" ht="13.55" customHeight="1">
+      <c r="A41" t="s" s="73">
+        <v>85</v>
+      </c>
+      <c r="B41" s="74"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="14"/>
+    </row>
+    <row r="42" ht="14" customHeight="1">
+      <c r="A42" t="s" s="33">
+        <v>59</v>
+      </c>
+      <c r="B42" s="50"/>
+      <c r="C42" t="s" s="15">
+        <v>11</v>
+      </c>
+      <c r="D42" t="s" s="16">
+        <v>12</v>
+      </c>
+      <c r="E42" t="s" s="16">
+        <v>60</v>
+      </c>
+      <c r="F42" s="48"/>
+      <c r="G42" t="s" s="11">
+        <v>85</v>
+      </c>
+      <c r="H42" t="s" s="33">
+        <v>59</v>
+      </c>
+      <c r="I42" s="22"/>
+    </row>
+    <row r="43" ht="91.5" customHeight="1">
+      <c r="A43" t="s" s="33">
+        <v>86</v>
+      </c>
+      <c r="B43" t="s" s="33">
+        <v>87</v>
+      </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="9"/>
+      <c r="E43" t="s" s="35">
         <v>45</v>
       </c>
-      <c r="F40" s="48"/>
-      <c r="G40" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="H40" s="69" t="s">
-        <v>81</v>
-      </c>
-      <c r="I40" s="13"/>
-    </row>
-    <row r="41" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="70" t="s">
-        <v>82</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="61" t="s">
-        <v>74</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="F41" s="71" t="s">
-        <v>84</v>
-      </c>
-      <c r="G41" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="H41" s="72" t="s">
-        <v>82</v>
-      </c>
-      <c r="I41" s="13"/>
-    </row>
-    <row r="42" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="73" t="s">
+      <c r="F43" s="48"/>
+      <c r="G43" t="s" s="11">
         <v>85</v>
       </c>
-      <c r="B42" s="74"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="38"/>
-      <c r="H42" s="38"/>
-      <c r="I42" s="14"/>
-    </row>
-    <row r="43" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="B43" s="50"/>
-      <c r="C43" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="F43" s="48"/>
-      <c r="G43" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="H43" s="33" t="s">
-        <v>59</v>
+      <c r="H43" t="s" s="33">
+        <v>86</v>
       </c>
       <c r="I43" s="22"/>
     </row>
-    <row r="44" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="B44" s="33" t="s">
-        <v>87</v>
+    <row r="44" ht="14" customHeight="1">
+      <c r="A44" t="s" s="33">
+        <v>88</v>
+      </c>
+      <c r="B44" t="s" s="33">
+        <v>89</v>
       </c>
       <c r="C44" s="13"/>
       <c r="D44" s="9"/>
-      <c r="E44" s="35" t="s">
+      <c r="E44" t="s" s="35">
         <v>45</v>
       </c>
       <c r="F44" s="48"/>
-      <c r="G44" s="11" t="s">
+      <c r="G44" t="s" s="11">
         <v>85</v>
       </c>
-      <c r="H44" s="33" t="s">
-        <v>86</v>
+      <c r="H44" t="s" s="33">
+        <v>88</v>
       </c>
       <c r="I44" s="22"/>
     </row>
-    <row r="45" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" s="33" t="s">
-        <v>89</v>
+    <row r="45" ht="14" customHeight="1">
+      <c r="A45" t="s" s="33">
+        <v>90</v>
+      </c>
+      <c r="B45" t="s" s="33">
+        <v>91</v>
       </c>
       <c r="C45" s="13"/>
       <c r="D45" s="9"/>
-      <c r="E45" s="35" t="s">
+      <c r="E45" t="s" s="35">
         <v>45</v>
       </c>
       <c r="F45" s="48"/>
-      <c r="G45" s="11" t="s">
+      <c r="G45" t="s" s="11">
         <v>85</v>
       </c>
-      <c r="H45" s="33" t="s">
-        <v>88</v>
+      <c r="H45" t="s" s="33">
+        <v>90</v>
       </c>
       <c r="I45" s="22"/>
     </row>
-    <row r="46" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" s="33" t="s">
-        <v>91</v>
+    <row r="46" ht="14" customHeight="1">
+      <c r="A46" t="s" s="33">
+        <v>92</v>
+      </c>
+      <c r="B46" t="s" s="33">
+        <v>93</v>
       </c>
       <c r="C46" s="13"/>
       <c r="D46" s="9"/>
-      <c r="E46" s="35" t="s">
+      <c r="E46" t="s" s="35">
         <v>45</v>
       </c>
       <c r="F46" s="48"/>
-      <c r="G46" s="11" t="s">
+      <c r="G46" t="s" s="11">
         <v>85</v>
       </c>
-      <c r="H46" s="33" t="s">
-        <v>90</v>
+      <c r="H46" t="s" s="33">
+        <v>92</v>
       </c>
       <c r="I46" s="22"/>
     </row>
-    <row r="47" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="B47" s="33" t="s">
-        <v>93</v>
+    <row r="47" ht="14" customHeight="1">
+      <c r="A47" t="s" s="33">
+        <v>94</v>
+      </c>
+      <c r="B47" t="s" s="33">
+        <v>95</v>
       </c>
       <c r="C47" s="13"/>
       <c r="D47" s="9"/>
-      <c r="E47" s="35" t="s">
+      <c r="E47" t="s" s="35">
         <v>45</v>
       </c>
       <c r="F47" s="48"/>
-      <c r="G47" s="11" t="s">
+      <c r="G47" t="s" s="11">
         <v>85</v>
       </c>
-      <c r="H47" s="33" t="s">
-        <v>92</v>
+      <c r="H47" t="s" s="33">
+        <v>94</v>
       </c>
       <c r="I47" s="22"/>
     </row>
-    <row r="48" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="B48" s="33" t="s">
-        <v>95</v>
-      </c>
+    <row r="48" ht="14" customHeight="1">
+      <c r="A48" t="s" s="6">
+        <v>96</v>
+      </c>
+      <c r="B48" s="50"/>
       <c r="C48" s="13"/>
       <c r="D48" s="9"/>
-      <c r="E48" s="35" t="s">
+      <c r="E48" t="s" s="35">
         <v>45</v>
       </c>
-      <c r="F48" s="48"/>
-      <c r="G48" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="H48" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="I48" s="22"/>
-    </row>
-    <row r="49" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+      <c r="F48" s="38"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="25"/>
+      <c r="I48" s="14"/>
+    </row>
+    <row r="49" ht="30.75" customHeight="1">
+      <c r="A49" t="s" s="33">
+        <v>97</v>
+      </c>
+      <c r="B49" s="50"/>
+      <c r="C49" t="s" s="15">
+        <v>11</v>
+      </c>
+      <c r="D49" t="s" s="16">
+        <v>12</v>
+      </c>
+      <c r="E49" t="s" s="75">
+        <v>60</v>
+      </c>
+      <c r="F49" s="11"/>
+      <c r="G49" t="s" s="60">
         <v>96</v>
       </c>
-      <c r="B49" s="50"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="F49" s="38"/>
-      <c r="G49" s="25"/>
-      <c r="H49" s="25"/>
-      <c r="I49" s="14"/>
-    </row>
-    <row r="50" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
+      <c r="H49" t="s" s="76">
         <v>97</v>
       </c>
-      <c r="B50" s="50"/>
-      <c r="C50" s="15" t="s">
+      <c r="I49" s="22"/>
+    </row>
+    <row r="50" ht="30.75" customHeight="1">
+      <c r="A50" t="s" s="33">
+        <v>98</v>
+      </c>
+      <c r="B50" s="34"/>
+      <c r="C50" t="s" s="15">
         <v>11</v>
       </c>
-      <c r="D50" s="16" t="s">
+      <c r="D50" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="E50" s="75" t="s">
-        <v>60</v>
-      </c>
-      <c r="F50" s="11"/>
-      <c r="G50" s="60" t="s">
+      <c r="E50" t="s" s="77">
+        <v>99</v>
+      </c>
+      <c r="F50" t="s" s="78">
+        <v>100</v>
+      </c>
+      <c r="G50" t="s" s="60">
         <v>96</v>
       </c>
-      <c r="H50" s="76" t="s">
-        <v>97</v>
+      <c r="H50" t="s" s="33">
+        <v>101</v>
       </c>
       <c r="I50" s="22"/>
     </row>
-    <row r="51" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="33" t="s">
-        <v>98</v>
+    <row r="51" ht="30.75" customHeight="1">
+      <c r="A51" t="s" s="33">
+        <v>96</v>
       </c>
       <c r="B51" s="34"/>
-      <c r="C51" s="15" t="s">
+      <c r="C51" t="s" s="79">
         <v>11</v>
       </c>
-      <c r="D51" s="16" t="s">
+      <c r="D51" t="s" s="80">
         <v>12</v>
       </c>
-      <c r="E51" s="77" t="s">
-        <v>99</v>
-      </c>
-      <c r="F51" s="78" t="s">
-        <v>100</v>
-      </c>
-      <c r="G51" s="60" t="s">
+      <c r="E51" t="s" s="81">
+        <v>102</v>
+      </c>
+      <c r="F51" s="82"/>
+      <c r="G51" t="s" s="60">
         <v>96</v>
       </c>
-      <c r="H51" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="I51" s="22"/>
-    </row>
-    <row r="52" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="B52" s="34"/>
-      <c r="C52" s="79" t="s">
-        <v>11</v>
-      </c>
-      <c r="D52" s="80" t="s">
-        <v>12</v>
-      </c>
-      <c r="E52" s="81" t="s">
-        <v>102</v>
-      </c>
-      <c r="F52" s="82"/>
-      <c r="G52" s="60" t="s">
-        <v>96</v>
-      </c>
-      <c r="H52" s="33" t="s">
+      <c r="H51" t="s" s="33">
         <v>103</v>
       </c>
-      <c r="I52" s="83"/>
+      <c r="I51" s="83"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G4" r:id="rId1" display="Company" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G5:G9" r:id="rId2" display="Company" xr:uid="{0CA84632-DE5E-447F-A0A5-EBCF9541770A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -3229,57 +3266,56 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="38.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="42.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="27.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="38.1719" style="84" customWidth="1"/>
+    <col min="2" max="2" width="42.3516" style="84" customWidth="1"/>
+    <col min="3" max="3" width="13.6719" style="84" customWidth="1"/>
+    <col min="4" max="4" width="23.3516" style="84" customWidth="1"/>
+    <col min="5" max="5" width="28" style="84" customWidth="1"/>
+    <col min="6" max="6" width="31.3516" style="84" customWidth="1"/>
+    <col min="7" max="7" width="26.3516" style="84" customWidth="1"/>
+    <col min="8" max="8" width="16.5" style="84" customWidth="1"/>
+    <col min="9" max="9" width="27.5" style="84" customWidth="1"/>
+    <col min="10" max="10" width="13.6719" style="84" customWidth="1"/>
+    <col min="11" max="16384" width="8.85156" style="84" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="13.55" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" t="s" s="2">
         <v>104</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="G1" s="84"/>
-      <c r="H1" s="85" t="s">
+      <c r="G1" s="85"/>
+      <c r="H1" t="s" s="86">
         <v>5</v>
       </c>
-      <c r="I1" s="86" t="s">
+      <c r="I1" t="s" s="87">
         <v>6</v>
       </c>
-      <c r="J1" s="85" t="s">
+      <c r="J1" t="s" s="86">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" ht="13.55" customHeight="1">
+      <c r="A2" t="s" s="6">
         <v>8</v>
       </c>
       <c r="B2" s="7"/>
@@ -3292,8 +3328,8 @@
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="87" t="s">
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="s" s="88">
         <v>9</v>
       </c>
       <c r="B3" s="12"/>
@@ -3306,164 +3342,164 @@
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="s" s="11">
         <v>10</v>
       </c>
       <c r="B4" s="12"/>
-      <c r="C4" s="15" t="s">
+      <c r="C4" t="s" s="15">
         <v>105</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" t="s" s="17">
         <v>11</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" t="s" s="16">
         <v>13</v>
       </c>
       <c r="G4" s="9"/>
-      <c r="H4" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="18" t="s">
+      <c r="H4" t="s" s="17">
+        <v>106</v>
+      </c>
+      <c r="I4" t="s" s="18">
         <v>15</v>
       </c>
       <c r="J4" s="9"/>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" t="s" s="11">
         <v>16</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="15" t="s">
+      <c r="C5" t="s" s="15">
         <v>105</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" t="s" s="17">
         <v>11</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" t="s" s="17">
         <v>17</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="18" t="s">
+      <c r="H5" t="s" s="17">
+        <v>106</v>
+      </c>
+      <c r="I5" t="s" s="18">
         <v>18</v>
       </c>
       <c r="J5" s="9"/>
     </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" t="s" s="11">
         <v>19</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="15" t="s">
+      <c r="C6" t="s" s="15">
         <v>105</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" t="s" s="17">
         <v>11</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" t="s" s="16">
         <v>20</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="18" t="s">
+      <c r="H6" t="s" s="17">
+        <v>106</v>
+      </c>
+      <c r="I6" t="s" s="18">
         <v>21</v>
       </c>
       <c r="J6" s="9"/>
     </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" t="s" s="11">
         <v>22</v>
       </c>
       <c r="B7" s="12"/>
-      <c r="C7" s="15" t="s">
+      <c r="C7" t="s" s="15">
         <v>105</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" t="s" s="17">
         <v>11</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" t="s" s="17">
         <v>23</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="18" t="s">
+      <c r="H7" t="s" s="17">
+        <v>106</v>
+      </c>
+      <c r="I7" t="s" s="18">
         <v>24</v>
       </c>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" t="s" s="11">
         <v>25</v>
       </c>
       <c r="B8" s="12"/>
-      <c r="C8" s="15" t="s">
+      <c r="C8" t="s" s="15">
         <v>105</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" t="s" s="17">
         <v>11</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" t="s" s="16">
         <v>26</v>
       </c>
       <c r="G8" s="9"/>
-      <c r="H8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="19" t="s">
+      <c r="H8" t="s" s="17">
+        <v>106</v>
+      </c>
+      <c r="I8" t="s" s="19">
         <v>27</v>
       </c>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+    <row r="9" ht="14" customHeight="1">
+      <c r="A9" t="s" s="11">
         <v>28</v>
       </c>
       <c r="B9" s="20"/>
-      <c r="C9" s="15" t="s">
+      <c r="C9" t="s" s="15">
         <v>105</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" t="s" s="17">
         <v>11</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" t="s" s="16">
         <v>29</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" t="s" s="16">
         <v>30</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="11" t="s">
+      <c r="H9" t="s" s="21">
+        <v>106</v>
+      </c>
+      <c r="I9" t="s" s="11">
         <v>28</v>
       </c>
       <c r="J9" s="13"/>
     </row>
-    <row r="10" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" t="s" s="23">
         <v>32</v>
       </c>
       <c r="B10" s="24"/>
@@ -3476,220 +3512,220 @@
       <c r="I10" s="25"/>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+    <row r="11" ht="14" customHeight="1">
+      <c r="A11" t="s" s="33">
         <v>38</v>
       </c>
       <c r="B11" s="34"/>
-      <c r="C11" s="15" t="s">
+      <c r="C11" t="s" s="15">
         <v>80</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" t="s" s="17">
         <v>33</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" t="s" s="16">
         <v>34</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" t="s" s="16">
         <v>39</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" t="s" s="17">
         <v>40</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" t="s" s="21">
         <v>36</v>
       </c>
-      <c r="I11" s="33" t="s">
+      <c r="I11" t="s" s="33">
         <v>38</v>
       </c>
       <c r="J11" s="13"/>
     </row>
-    <row r="12" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+    <row r="12" ht="14" customHeight="1">
+      <c r="A12" t="s" s="33">
         <v>41</v>
       </c>
       <c r="B12" s="34"/>
       <c r="C12" s="13"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="16" t="s">
+      <c r="F12" t="s" s="16">
         <v>39</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" t="s" s="17">
         <v>42</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="H12" t="s" s="21">
         <v>36</v>
       </c>
-      <c r="I12" s="33" t="s">
+      <c r="I12" t="s" s="33">
         <v>41</v>
       </c>
       <c r="J12" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+    <row r="13" ht="14" customHeight="1">
+      <c r="A13" t="s" s="33">
         <v>43</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" t="s" s="33">
         <v>44</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
-      <c r="F13" s="88" t="s">
+      <c r="F13" t="s" s="89">
         <v>45</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="21" t="s">
+      <c r="H13" t="s" s="21">
         <v>36</v>
       </c>
-      <c r="I13" s="33" t="s">
+      <c r="I13" t="s" s="33">
         <v>43</v>
       </c>
       <c r="J13" s="13"/>
     </row>
-    <row r="14" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+    <row r="14" ht="14" customHeight="1">
+      <c r="A14" t="s" s="33">
         <v>46</v>
       </c>
       <c r="B14" s="34"/>
-      <c r="C14" s="15" t="s">
+      <c r="C14" t="s" s="15">
         <v>80</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" t="s" s="17">
         <v>33</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" t="s" s="16">
         <v>34</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" t="s" s="16">
         <v>47</v>
       </c>
       <c r="G14" s="9"/>
-      <c r="H14" s="21" t="s">
+      <c r="H14" t="s" s="21">
         <v>36</v>
       </c>
-      <c r="I14" s="33" t="s">
+      <c r="I14" t="s" s="33">
         <v>46</v>
       </c>
       <c r="J14" s="13"/>
     </row>
-    <row r="15" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+    <row r="15" ht="14" customHeight="1">
+      <c r="A15" t="s" s="33">
         <v>48</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" t="s" s="33">
         <v>49</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
-      <c r="F15" s="88" t="s">
+      <c r="F15" t="s" s="89">
         <v>45</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="21" t="s">
+      <c r="H15" t="s" s="21">
         <v>36</v>
       </c>
-      <c r="I15" s="33" t="s">
+      <c r="I15" t="s" s="33">
         <v>48</v>
       </c>
       <c r="J15" s="13"/>
     </row>
-    <row r="16" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+    <row r="16" ht="14" customHeight="1">
+      <c r="A16" t="s" s="33">
         <v>50</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" t="s" s="11">
         <v>51</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="88" t="s">
+      <c r="F16" t="s" s="89">
         <v>45</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="21" t="s">
+      <c r="H16" t="s" s="21">
         <v>36</v>
       </c>
-      <c r="I16" s="33" t="s">
+      <c r="I16" t="s" s="33">
         <v>50</v>
       </c>
       <c r="J16" s="13"/>
     </row>
-    <row r="17" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+    <row r="17" ht="14" customHeight="1">
+      <c r="A17" t="s" s="33">
         <v>52</v>
       </c>
       <c r="B17" s="34"/>
-      <c r="C17" s="15" t="s">
+      <c r="C17" t="s" s="15">
         <v>80</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" t="s" s="17">
         <v>33</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" t="s" s="16">
         <v>34</v>
       </c>
-      <c r="F17" s="89" t="s">
+      <c r="F17" t="s" s="90">
         <v>53</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="21" t="s">
+      <c r="H17" t="s" s="21">
         <v>36</v>
       </c>
-      <c r="I17" s="33" t="s">
+      <c r="I17" t="s" s="33">
         <v>52</v>
       </c>
       <c r="J17" s="13"/>
     </row>
-    <row r="18" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
+    <row r="18" ht="14" customHeight="1">
+      <c r="A18" t="s" s="33">
         <v>54</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" t="s" s="33">
         <v>55</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
-      <c r="F18" s="88" t="s">
+      <c r="F18" t="s" s="89">
         <v>45</v>
       </c>
       <c r="G18" s="9"/>
-      <c r="H18" s="21" t="s">
+      <c r="H18" t="s" s="21">
         <v>36</v>
       </c>
-      <c r="I18" s="33" t="s">
+      <c r="I18" t="s" s="33">
         <v>54</v>
       </c>
       <c r="J18" s="13"/>
     </row>
-    <row r="19" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+    <row r="19" ht="14" customHeight="1">
+      <c r="A19" t="s" s="33">
         <v>56</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" t="s" s="33">
         <v>57</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
-      <c r="F19" s="88" t="s">
+      <c r="F19" t="s" s="89">
         <v>45</v>
       </c>
       <c r="G19" s="9"/>
-      <c r="H19" s="21" t="s">
+      <c r="H19" t="s" s="21">
         <v>36</v>
       </c>
-      <c r="I19" s="33" t="s">
+      <c r="I19" t="s" s="33">
         <v>56</v>
       </c>
       <c r="J19" s="13"/>
     </row>
-    <row r="20" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
+    <row r="20" ht="13.55" customHeight="1">
+      <c r="A20" t="s" s="37">
         <v>58</v>
       </c>
       <c r="B20" s="24"/>
@@ -3702,34 +3738,34 @@
       <c r="I20" s="25"/>
       <c r="J20" s="9"/>
     </row>
-    <row r="21" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
+    <row r="21" ht="14" customHeight="1">
+      <c r="A21" t="s" s="33">
         <v>59</v>
       </c>
       <c r="B21" s="50"/>
-      <c r="C21" s="15" t="s">
+      <c r="C21" t="s" s="15">
         <v>105</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" t="s" s="17">
         <v>11</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" t="s" s="16">
         <v>60</v>
       </c>
       <c r="G21" s="48"/>
-      <c r="H21" s="87" t="s">
+      <c r="H21" t="s" s="88">
         <v>61</v>
       </c>
-      <c r="I21" s="33" t="s">
+      <c r="I21" t="s" s="33">
         <v>59</v>
       </c>
       <c r="J21" s="13"/>
     </row>
-    <row r="22" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="87" t="s">
+    <row r="22" ht="13.55" customHeight="1">
+      <c r="A22" t="s" s="88">
         <v>61</v>
       </c>
       <c r="B22" s="50"/>
@@ -3742,156 +3778,156 @@
       <c r="I22" s="25"/>
       <c r="J22" s="9"/>
     </row>
-    <row r="23" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="33" t="s">
+    <row r="23" ht="14" customHeight="1">
+      <c r="A23" t="s" s="33">
         <v>64</v>
       </c>
       <c r="B23" s="34"/>
-      <c r="C23" s="15" t="s">
+      <c r="C23" t="s" s="15">
         <v>80</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" t="s" s="17">
         <v>33</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" t="s" s="16">
         <v>34</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" t="s" s="16">
         <v>39</v>
       </c>
       <c r="G23" s="48"/>
-      <c r="H23" s="87" t="s">
+      <c r="H23" t="s" s="88">
         <v>61</v>
       </c>
-      <c r="I23" s="33" t="s">
+      <c r="I23" t="s" s="33">
         <v>64</v>
       </c>
       <c r="J23" s="13"/>
     </row>
-    <row r="24" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="33" t="s">
+    <row r="24" ht="30.75" customHeight="1">
+      <c r="A24" t="s" s="33">
         <v>66</v>
       </c>
       <c r="B24" s="34"/>
       <c r="C24" s="13"/>
       <c r="D24" s="9"/>
-      <c r="E24" s="17" t="s">
+      <c r="E24" t="s" s="17">
         <v>67</v>
       </c>
       <c r="F24" s="9"/>
-      <c r="G24" s="49" t="s">
+      <c r="G24" t="s" s="49">
         <v>68</v>
       </c>
-      <c r="H24" s="87" t="s">
+      <c r="H24" t="s" s="88">
         <v>61</v>
       </c>
-      <c r="I24" s="33" t="s">
+      <c r="I24" t="s" s="33">
         <v>66</v>
       </c>
       <c r="J24" s="13"/>
     </row>
-    <row r="25" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+    <row r="25" ht="14" customHeight="1">
+      <c r="A25" t="s" s="33">
         <v>43</v>
       </c>
-      <c r="B25" s="33" t="s">
+      <c r="B25" t="s" s="33">
         <v>44</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
-      <c r="F25" s="88" t="s">
+      <c r="F25" t="s" s="89">
         <v>45</v>
       </c>
       <c r="G25" s="48"/>
-      <c r="H25" s="87" t="s">
+      <c r="H25" t="s" s="88">
         <v>61</v>
       </c>
-      <c r="I25" s="33" t="s">
+      <c r="I25" t="s" s="33">
         <v>43</v>
       </c>
       <c r="J25" s="13"/>
     </row>
-    <row r="26" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="33" t="s">
+    <row r="26" ht="14" customHeight="1">
+      <c r="A26" t="s" s="33">
         <v>46</v>
       </c>
       <c r="B26" s="34"/>
-      <c r="C26" s="15" t="s">
+      <c r="C26" t="s" s="15">
         <v>80</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" t="s" s="17">
         <v>33</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" t="s" s="16">
         <v>34</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="F26" t="s" s="16">
         <v>47</v>
       </c>
       <c r="G26" s="48"/>
-      <c r="H26" s="87" t="s">
+      <c r="H26" t="s" s="88">
         <v>61</v>
       </c>
-      <c r="I26" s="33" t="s">
+      <c r="I26" t="s" s="33">
         <v>46</v>
       </c>
       <c r="J26" s="13"/>
     </row>
-    <row r="27" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
+    <row r="27" ht="14" customHeight="1">
+      <c r="A27" t="s" s="33">
         <v>69</v>
       </c>
       <c r="B27" s="34"/>
-      <c r="C27" s="15" t="s">
+      <c r="C27" t="s" s="15">
         <v>80</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" t="s" s="17">
         <v>33</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" t="s" s="16">
         <v>34</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" t="s" s="16">
         <v>70</v>
       </c>
       <c r="G27" s="48"/>
-      <c r="H27" s="87" t="s">
+      <c r="H27" t="s" s="88">
         <v>61</v>
       </c>
-      <c r="I27" s="33" t="s">
+      <c r="I27" t="s" s="33">
         <v>69</v>
       </c>
       <c r="J27" s="13"/>
     </row>
-    <row r="28" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="33" t="s">
+    <row r="28" ht="14" customHeight="1">
+      <c r="A28" t="s" s="33">
         <v>71</v>
       </c>
       <c r="B28" s="34"/>
-      <c r="C28" s="15" t="s">
+      <c r="C28" t="s" s="15">
         <v>80</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="D28" t="s" s="17">
         <v>33</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" t="s" s="16">
         <v>34</v>
       </c>
-      <c r="F28" s="16" t="s">
+      <c r="F28" t="s" s="16">
         <v>72</v>
       </c>
       <c r="G28" s="48"/>
-      <c r="H28" s="87" t="s">
+      <c r="H28" t="s" s="88">
         <v>61</v>
       </c>
-      <c r="I28" s="33" t="s">
+      <c r="I28" t="s" s="33">
         <v>71</v>
       </c>
       <c r="J28" s="13"/>
     </row>
-    <row r="29" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="87" t="s">
+    <row r="29" ht="13.55" customHeight="1">
+      <c r="A29" t="s" s="88">
         <v>73</v>
       </c>
       <c r="B29" s="20"/>
@@ -3904,37 +3940,37 @@
       <c r="I29" s="25"/>
       <c r="J29" s="9"/>
     </row>
-    <row r="30" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="33" t="s">
+    <row r="30" ht="37.5" customHeight="1">
+      <c r="A30" t="s" s="33">
         <v>64</v>
       </c>
       <c r="B30" s="20"/>
-      <c r="C30" s="15" t="s">
+      <c r="C30" t="s" s="15">
         <v>80</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D30" t="s" s="17">
         <v>33</v>
       </c>
-      <c r="E30" s="61" t="s">
-        <v>106</v>
-      </c>
-      <c r="F30" s="16" t="s">
+      <c r="E30" t="s" s="61">
+        <v>107</v>
+      </c>
+      <c r="F30" t="s" s="16">
         <v>39</v>
       </c>
       <c r="G30" s="48"/>
-      <c r="H30" s="87" t="s">
+      <c r="H30" t="s" s="88">
         <v>73</v>
       </c>
-      <c r="I30" s="33" t="s">
+      <c r="I30" t="s" s="33">
         <v>64</v>
       </c>
       <c r="J30" s="13"/>
     </row>
-    <row r="31" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
+    <row r="31" ht="13.55" customHeight="1">
+      <c r="A31" t="s" s="33">
         <v>66</v>
       </c>
-      <c r="B31" s="33" t="s">
+      <c r="B31" t="s" s="33">
         <v>77</v>
       </c>
       <c r="C31" s="13"/>
@@ -3942,116 +3978,116 @@
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="48"/>
-      <c r="H31" s="87" t="s">
+      <c r="H31" t="s" s="88">
         <v>73</v>
       </c>
-      <c r="I31" s="33" t="s">
+      <c r="I31" t="s" s="33">
         <v>66</v>
       </c>
       <c r="J31" s="13"/>
     </row>
-    <row r="32" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="s">
+    <row r="32" ht="14" customHeight="1">
+      <c r="A32" t="s" s="33">
         <v>43</v>
       </c>
-      <c r="B32" s="60" t="s">
+      <c r="B32" t="s" s="60">
         <v>78</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
-      <c r="F32" s="88" t="s">
+      <c r="F32" t="s" s="89">
         <v>45</v>
       </c>
       <c r="G32" s="48"/>
-      <c r="H32" s="87" t="s">
+      <c r="H32" t="s" s="88">
         <v>73</v>
       </c>
-      <c r="I32" s="33" t="s">
+      <c r="I32" t="s" s="33">
         <v>43</v>
       </c>
       <c r="J32" s="13"/>
     </row>
-    <row r="33" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+    <row r="33" ht="37.5" customHeight="1">
+      <c r="A33" t="s" s="33">
         <v>46</v>
       </c>
       <c r="B33" s="50"/>
-      <c r="C33" s="15" t="s">
+      <c r="C33" t="s" s="15">
         <v>80</v>
       </c>
-      <c r="D33" s="17" t="s">
+      <c r="D33" t="s" s="17">
         <v>33</v>
       </c>
-      <c r="E33" s="61" t="s">
-        <v>106</v>
-      </c>
-      <c r="F33" s="17" t="s">
+      <c r="E33" t="s" s="61">
+        <v>107</v>
+      </c>
+      <c r="F33" t="s" s="17">
         <v>47</v>
       </c>
       <c r="G33" s="48"/>
-      <c r="H33" s="87" t="s">
+      <c r="H33" t="s" s="88">
         <v>73</v>
       </c>
-      <c r="I33" s="33" t="s">
+      <c r="I33" t="s" s="33">
         <v>46</v>
       </c>
       <c r="J33" s="13"/>
     </row>
-    <row r="34" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
+    <row r="34" ht="37.5" customHeight="1">
+      <c r="A34" t="s" s="33">
         <v>69</v>
       </c>
       <c r="B34" s="50"/>
-      <c r="C34" s="15" t="s">
+      <c r="C34" t="s" s="15">
         <v>80</v>
       </c>
-      <c r="D34" s="17" t="s">
+      <c r="D34" t="s" s="17">
         <v>33</v>
       </c>
-      <c r="E34" s="61" t="s">
-        <v>106</v>
-      </c>
-      <c r="F34" s="16" t="s">
+      <c r="E34" t="s" s="61">
+        <v>107</v>
+      </c>
+      <c r="F34" t="s" s="16">
         <v>70</v>
       </c>
       <c r="G34" s="48"/>
-      <c r="H34" s="87" t="s">
+      <c r="H34" t="s" s="88">
         <v>73</v>
       </c>
-      <c r="I34" s="33" t="s">
+      <c r="I34" t="s" s="33">
         <v>69</v>
       </c>
       <c r="J34" s="13"/>
     </row>
-    <row r="35" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="33" t="s">
+    <row r="35" ht="37.5" customHeight="1">
+      <c r="A35" t="s" s="33">
         <v>71</v>
       </c>
       <c r="B35" s="20"/>
-      <c r="C35" s="15" t="s">
+      <c r="C35" t="s" s="15">
         <v>80</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="D35" t="s" s="17">
         <v>33</v>
       </c>
-      <c r="E35" s="61" t="s">
-        <v>106</v>
-      </c>
-      <c r="F35" s="16" t="s">
+      <c r="E35" t="s" s="61">
+        <v>107</v>
+      </c>
+      <c r="F35" t="s" s="16">
         <v>72</v>
       </c>
       <c r="G35" s="48"/>
-      <c r="H35" s="87" t="s">
+      <c r="H35" t="s" s="88">
         <v>73</v>
       </c>
-      <c r="I35" s="33" t="s">
+      <c r="I35" t="s" s="33">
         <v>71</v>
       </c>
       <c r="J35" s="13"/>
     </row>
-    <row r="36" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+    <row r="36" ht="13.55" customHeight="1">
+      <c r="A36" t="s" s="6">
         <v>85</v>
       </c>
       <c r="B36" s="50"/>
@@ -4064,151 +4100,151 @@
       <c r="I36" s="25"/>
       <c r="J36" s="9"/>
     </row>
-    <row r="37" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="33" t="s">
+    <row r="37" ht="14" customHeight="1">
+      <c r="A37" t="s" s="33">
         <v>59</v>
       </c>
       <c r="B37" s="50"/>
-      <c r="C37" s="15" t="s">
+      <c r="C37" t="s" s="15">
         <v>105</v>
       </c>
-      <c r="D37" s="17" t="s">
+      <c r="D37" t="s" s="17">
         <v>11</v>
       </c>
-      <c r="E37" s="16" t="s">
+      <c r="E37" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="F37" s="16" t="s">
+      <c r="F37" t="s" s="16">
         <v>60</v>
       </c>
       <c r="G37" s="48"/>
-      <c r="H37" s="11" t="s">
+      <c r="H37" t="s" s="11">
         <v>85</v>
       </c>
-      <c r="I37" s="33" t="s">
+      <c r="I37" t="s" s="33">
         <v>59</v>
       </c>
       <c r="J37" s="13"/>
     </row>
-    <row r="38" spans="1:10" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="33" t="s">
+    <row r="38" ht="91.5" customHeight="1">
+      <c r="A38" t="s" s="33">
         <v>86</v>
       </c>
-      <c r="B38" s="33" t="s">
+      <c r="B38" t="s" s="33">
         <v>87</v>
       </c>
       <c r="C38" s="13"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
-      <c r="F38" s="88" t="s">
+      <c r="F38" t="s" s="89">
         <v>45</v>
       </c>
       <c r="G38" s="48"/>
-      <c r="H38" s="11" t="s">
+      <c r="H38" t="s" s="11">
         <v>85</v>
       </c>
-      <c r="I38" s="33" t="s">
+      <c r="I38" t="s" s="33">
         <v>86</v>
       </c>
       <c r="J38" s="13"/>
     </row>
-    <row r="39" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="33" t="s">
+    <row r="39" ht="14" customHeight="1">
+      <c r="A39" t="s" s="33">
         <v>88</v>
       </c>
-      <c r="B39" s="33" t="s">
+      <c r="B39" t="s" s="33">
         <v>89</v>
       </c>
       <c r="C39" s="13"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
-      <c r="F39" s="88" t="s">
+      <c r="F39" t="s" s="89">
         <v>45</v>
       </c>
       <c r="G39" s="48"/>
-      <c r="H39" s="11" t="s">
+      <c r="H39" t="s" s="11">
         <v>85</v>
       </c>
-      <c r="I39" s="33" t="s">
+      <c r="I39" t="s" s="33">
         <v>88</v>
       </c>
       <c r="J39" s="13"/>
     </row>
-    <row r="40" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="33" t="s">
+    <row r="40" ht="14" customHeight="1">
+      <c r="A40" t="s" s="33">
         <v>90</v>
       </c>
-      <c r="B40" s="33" t="s">
+      <c r="B40" t="s" s="33">
         <v>91</v>
       </c>
       <c r="C40" s="13"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
-      <c r="F40" s="88" t="s">
+      <c r="F40" t="s" s="89">
         <v>45</v>
       </c>
       <c r="G40" s="48"/>
-      <c r="H40" s="11" t="s">
+      <c r="H40" t="s" s="11">
         <v>85</v>
       </c>
-      <c r="I40" s="33" t="s">
+      <c r="I40" t="s" s="33">
         <v>90</v>
       </c>
       <c r="J40" s="13"/>
     </row>
-    <row r="41" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="33" t="s">
+    <row r="41" ht="14" customHeight="1">
+      <c r="A41" t="s" s="33">
         <v>92</v>
       </c>
-      <c r="B41" s="33" t="s">
+      <c r="B41" t="s" s="33">
         <v>93</v>
       </c>
       <c r="C41" s="13"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
-      <c r="F41" s="88" t="s">
+      <c r="F41" t="s" s="89">
         <v>45</v>
       </c>
       <c r="G41" s="48"/>
-      <c r="H41" s="11" t="s">
+      <c r="H41" t="s" s="11">
         <v>85</v>
       </c>
-      <c r="I41" s="33" t="s">
+      <c r="I41" t="s" s="33">
         <v>92</v>
       </c>
       <c r="J41" s="13"/>
     </row>
-    <row r="42" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="33" t="s">
+    <row r="42" ht="14" customHeight="1">
+      <c r="A42" t="s" s="33">
         <v>94</v>
       </c>
-      <c r="B42" s="33" t="s">
+      <c r="B42" t="s" s="33">
         <v>95</v>
       </c>
       <c r="C42" s="13"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
-      <c r="F42" s="88" t="s">
+      <c r="F42" t="s" s="89">
         <v>45</v>
       </c>
       <c r="G42" s="48"/>
-      <c r="H42" s="11" t="s">
+      <c r="H42" t="s" s="11">
         <v>85</v>
       </c>
-      <c r="I42" s="33" t="s">
+      <c r="I42" t="s" s="33">
         <v>94</v>
       </c>
       <c r="J42" s="13"/>
     </row>
-    <row r="43" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+    <row r="43" ht="14" customHeight="1">
+      <c r="A43" t="s" s="6">
         <v>96</v>
       </c>
       <c r="B43" s="50"/>
       <c r="C43" s="13"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
-      <c r="F43" s="88" t="s">
+      <c r="F43" t="s" s="89">
         <v>45</v>
       </c>
       <c r="G43" s="38"/>
@@ -4216,95 +4252,95 @@
       <c r="I43" s="25"/>
       <c r="J43" s="9"/>
     </row>
-    <row r="44" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="33" t="s">
+    <row r="44" ht="30.75" customHeight="1">
+      <c r="A44" t="s" s="33">
         <v>97</v>
       </c>
       <c r="B44" s="50"/>
-      <c r="C44" s="15" t="s">
+      <c r="C44" t="s" s="15">
         <v>105</v>
       </c>
-      <c r="D44" s="17" t="s">
+      <c r="D44" t="s" s="17">
         <v>11</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="E44" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="F44" s="75" t="s">
+      <c r="F44" t="s" s="75">
         <v>60</v>
       </c>
       <c r="G44" s="11"/>
-      <c r="H44" s="60" t="s">
+      <c r="H44" t="s" s="60">
         <v>96</v>
       </c>
-      <c r="I44" s="76" t="s">
+      <c r="I44" t="s" s="76">
         <v>97</v>
       </c>
       <c r="J44" s="13"/>
     </row>
-    <row r="45" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="33" t="s">
+    <row r="45" ht="30.75" customHeight="1">
+      <c r="A45" t="s" s="33">
         <v>98</v>
       </c>
       <c r="B45" s="34"/>
-      <c r="C45" s="15" t="s">
+      <c r="C45" t="s" s="15">
         <v>105</v>
       </c>
-      <c r="D45" s="17" t="s">
+      <c r="D45" t="s" s="17">
         <v>11</v>
       </c>
-      <c r="E45" s="16" t="s">
+      <c r="E45" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="F45" s="90" t="s">
-        <v>107</v>
-      </c>
-      <c r="G45" s="91"/>
-      <c r="H45" s="60" t="s">
+      <c r="F45" t="s" s="91">
+        <v>108</v>
+      </c>
+      <c r="G45" s="92"/>
+      <c r="H45" t="s" s="60">
         <v>96</v>
       </c>
-      <c r="I45" s="33" t="s">
+      <c r="I45" t="s" s="33">
         <v>98</v>
       </c>
       <c r="J45" s="13"/>
     </row>
-    <row r="46" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="s">
+    <row r="46" ht="30.75" customHeight="1">
+      <c r="A46" t="s" s="33">
         <v>96</v>
       </c>
       <c r="B46" s="34"/>
-      <c r="C46" s="15" t="s">
+      <c r="C46" t="s" s="15">
         <v>105</v>
       </c>
-      <c r="D46" s="17" t="s">
+      <c r="D46" t="s" s="17">
         <v>11</v>
       </c>
-      <c r="E46" s="16" t="s">
+      <c r="E46" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="F46" s="89" t="s">
+      <c r="F46" t="s" s="90">
         <v>102</v>
       </c>
       <c r="G46" s="48"/>
-      <c r="H46" s="60" t="s">
+      <c r="H46" t="s" s="60">
         <v>96</v>
       </c>
-      <c r="I46" s="33" t="s">
+      <c r="I46" t="s" s="33">
         <v>96</v>
       </c>
       <c r="J46" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="H5" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="H6" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="H7" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="H8" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="H9" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="H4" r:id="rId1" location="" tooltip="" display="Company"/>
+    <hyperlink ref="H5" r:id="rId2" location="" tooltip="" display="Company"/>
+    <hyperlink ref="H6" r:id="rId3" location="" tooltip="" display="Company"/>
+    <hyperlink ref="H7" r:id="rId4" location="" tooltip="" display="Company"/>
+    <hyperlink ref="H8" r:id="rId5" location="" tooltip="" display="Company"/>
+    <hyperlink ref="H9" r:id="rId6" location="" tooltip="" display="Company"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Updated Form 11 hidden fields config
</commit_message>
<xml_diff>
--- a/Config Files/FORM-11_nodes_config.xlsx
+++ b/Config Files/FORM-11_nodes_config.xlsx
@@ -1,18 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCA Portal\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258F18CF-4CDB-487E-8C8F-CDF25BFEACB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet1-1" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1-1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$30</definedName>
+  </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="126">
   <si>
     <t>Field_Name</t>
   </si>
@@ -355,27 +367,63 @@
   <si>
     <t>BUSINESS_CLASS(hlf name is coming in xml)</t>
   </si>
+  <si>
+    <t>Hidden</t>
+  </si>
+  <si>
+    <t>DPartName</t>
+  </si>
+  <si>
+    <t>AppDate</t>
+  </si>
+  <si>
+    <t>CessDate</t>
+  </si>
+  <si>
+    <t>DFathHusName</t>
+  </si>
+  <si>
+    <t>CompanyAdd_C</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>Individuals,LLPs,Companies,Foreign LLPs,Foreign Companies,LLPs incorporated outside India,Companies incorporated outside India/
+Companies registered in Sikkim</t>
+  </si>
+  <si>
+    <t>CINorLLPIN</t>
+  </si>
+  <si>
+    <t>Logic</t>
+  </si>
+  <si>
+    <t>BodyCorpName</t>
+  </si>
+  <si>
+    <t>BodyCName</t>
+  </si>
+  <si>
+    <t>txtIndNOP,txtLLPNOP,txtCNOP,txtFLLPINOP,txtFCMPOP,txtLLPINOP,txtCINOP</t>
+  </si>
+  <si>
+    <t>txtIndNODP,txtLLPNODP,txtCNODP,txtFLLPINODP,txtFCMPODP,txtLLPINODP,txtCINODP</t>
+  </si>
+  <si>
+    <t>txtIndNODPRI,txtLLPNODPRI,txtCNODPRI,txtFLLPINOTHR,txtFCMPOTHR,txtLLPINODPRI,txtCINODPRI</t>
+  </si>
+  <si>
+    <t>txtTotIndividual,txtTotLLP,txtTotCompany,txtTotFLLPIN,txtTottxtFCMP,txtTotIncorporateOInd,txtTotCompOInd</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -395,19 +443,19 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="15"/>
       <name val="Courier New"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="19"/>
       <name val="Courier New"/>
@@ -428,7 +476,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="20"/>
       <name val="Courier New"/>
@@ -839,295 +887,164 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+  <cellXfs count="94">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="justify" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="justify" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="7" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="7" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="8" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1137,36 +1054,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffd8d8d8"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff92d050"/>
-      <rgbColor rgb="ff1d1d1c"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ff881280"/>
-      <rgbColor rgb="ff444444"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="fff8ff61"/>
-      <rgbColor rgb="ff7030a0"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="fffcff40"/>
-      <rgbColor rgb="fff9ff5a"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFD8D8D8"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FF92D050"/>
+      <rgbColor rgb="FF1D1D1C"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FF881280"/>
+      <rgbColor rgb="FF444444"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FFF8FF61"/>
+      <rgbColor rgb="FF7030A0"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFFCFF40"/>
+      <rgbColor rgb="FFF9FF5A"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -1368,7 +1334,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1386,7 +1352,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1415,7 +1381,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1440,7 +1406,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1465,7 +1431,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1490,7 +1456,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1515,7 +1481,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1540,7 +1506,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1565,7 +1531,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1590,7 +1556,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1615,7 +1581,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1628,9 +1594,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1647,7 +1619,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1665,7 +1637,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1690,7 +1662,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1715,7 +1687,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1740,7 +1712,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1765,7 +1737,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1790,7 +1762,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1815,7 +1787,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1840,7 +1812,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1865,7 +1837,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1890,7 +1862,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1903,9 +1875,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1919,7 +1897,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1937,7 +1915,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1966,7 +1944,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1991,7 +1969,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2016,7 +1994,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2041,7 +2019,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2066,7 +2044,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2091,7 +2069,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2116,7 +2094,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2141,7 +2119,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2166,7 +2144,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2179,65 +2157,75 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.1719" style="1" customWidth="1"/>
-    <col min="2" max="2" width="42.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.3516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28" style="1" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="105.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="33" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.3516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.1719" style="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6719" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="4"/>
-      <c r="G1" t="s" s="2">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s" s="5">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s" s="2">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="6">
+    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="7"/>
@@ -2249,8 +2237,8 @@
       <c r="H2" s="8"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="11">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="12"/>
@@ -2262,1038 +2250,1099 @@
       <c r="H3" s="9"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" ht="38.35" customHeight="1">
-      <c r="A4" t="s" s="11">
+    <row r="4" spans="1:9" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="12"/>
-      <c r="C4" t="s" s="15">
+      <c r="C4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s" s="16">
+      <c r="D4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s" s="16">
+      <c r="E4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s" s="18">
+      <c r="F4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G4" t="s" s="19">
+      <c r="G4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H4" t="s" s="20">
+      <c r="H4" s="19" t="s">
         <v>16</v>
       </c>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="11">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" t="s" s="15">
+      <c r="C5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s" s="16">
+      <c r="D5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="s" s="19">
+      <c r="E5" s="18" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="9"/>
-      <c r="G5" t="s" s="19">
+      <c r="G5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H5" t="s" s="20">
+      <c r="H5" s="19" t="s">
         <v>19</v>
       </c>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="11">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" t="s" s="15">
+      <c r="C6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s" s="16">
+      <c r="D6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="s" s="16">
+      <c r="E6" s="16" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="9"/>
-      <c r="G6" t="s" s="19">
+      <c r="G6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H6" t="s" s="20">
+      <c r="H6" s="19" t="s">
         <v>22</v>
       </c>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="11">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="12"/>
-      <c r="C7" t="s" s="15">
+      <c r="C7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s" s="16">
+      <c r="D7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s" s="19">
+      <c r="E7" s="18" t="s">
         <v>24</v>
       </c>
       <c r="F7" s="9"/>
-      <c r="G7" t="s" s="19">
+      <c r="G7" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H7" t="s" s="20">
+      <c r="H7" s="19" t="s">
         <v>25</v>
       </c>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="11">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="12"/>
-      <c r="C8" t="s" s="15">
+      <c r="C8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s" s="16">
+      <c r="D8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E8" t="s" s="16">
+      <c r="E8" s="16" t="s">
         <v>27</v>
       </c>
       <c r="F8" s="9"/>
-      <c r="G8" t="s" s="19">
+      <c r="G8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H8" t="s" s="21">
+      <c r="H8" s="20" t="s">
         <v>28</v>
       </c>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" ht="14" customHeight="1">
-      <c r="A9" t="s" s="11">
+    <row r="9" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" t="s" s="15">
+      <c r="B9" s="21"/>
+      <c r="C9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D9" t="s" s="16">
+      <c r="D9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E9" t="s" s="16">
+      <c r="E9" s="16" t="s">
         <v>30</v>
       </c>
       <c r="F9" s="9"/>
-      <c r="G9" t="s" s="23">
+      <c r="G9" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H9" t="s" s="11">
+      <c r="H9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="24"/>
-    </row>
-    <row r="10" ht="14" customHeight="1">
-      <c r="A10" t="s" s="11">
+      <c r="I9" s="23"/>
+    </row>
+    <row r="10" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" t="s" s="15">
+      <c r="B10" s="21"/>
+      <c r="C10" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s" s="16">
+      <c r="D10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E10" t="s" s="19">
+      <c r="E10" s="18" t="s">
         <v>31</v>
       </c>
       <c r="F10" s="9"/>
-      <c r="G10" t="s" s="23">
+      <c r="G10" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H10" t="s" s="11">
+      <c r="H10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="24"/>
-    </row>
-    <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" t="s" s="25">
+      <c r="I10" s="23"/>
+    </row>
+    <row r="11" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="26"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="27"/>
+      <c r="H11" s="26"/>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" ht="14" customHeight="1">
-      <c r="A12" t="s" s="28">
+    <row r="12" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" t="s" s="30">
+      <c r="B12" s="28"/>
+      <c r="C12" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="D12" t="s" s="31">
+      <c r="D12" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E12" t="s" s="31">
+      <c r="E12" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="32"/>
-      <c r="G12" t="s" s="33">
+      <c r="F12" s="31"/>
+      <c r="G12" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="H12" t="s" s="28">
+      <c r="H12" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="I12" s="34"/>
-    </row>
-    <row r="13" ht="14" customHeight="1">
-      <c r="A13" t="s" s="35">
+      <c r="I12" s="33"/>
+    </row>
+    <row r="13" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="36"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="13"/>
-      <c r="D13" t="s" s="16">
+      <c r="D13" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E13" t="s" s="16">
+      <c r="E13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F13" t="s" s="19">
+      <c r="F13" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G13" t="s" s="23">
+      <c r="G13" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H13" t="s" s="35">
+      <c r="H13" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="I13" s="24"/>
-    </row>
-    <row r="14" ht="14" customHeight="1">
-      <c r="A14" t="s" s="35">
+      <c r="I13" s="23"/>
+    </row>
+    <row r="14" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="36"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="13"/>
       <c r="D14" s="9"/>
-      <c r="E14" t="s" s="16">
+      <c r="E14" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F14" t="s" s="19">
+      <c r="F14" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G14" t="s" s="23">
+      <c r="G14" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H14" t="s" s="35">
+      <c r="H14" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="I14" s="24"/>
-    </row>
-    <row r="15" ht="14" customHeight="1">
-      <c r="A15" t="s" s="35">
+      <c r="I14" s="23"/>
+    </row>
+    <row r="15" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B15" t="s" s="35">
+      <c r="B15" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="9"/>
-      <c r="E15" t="s" s="37">
+      <c r="C15" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="36" t="s">
         <v>45</v>
       </c>
       <c r="F15" s="9"/>
-      <c r="G15" t="s" s="23">
+      <c r="G15" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H15" t="s" s="35">
+      <c r="H15" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="I15" s="24"/>
-    </row>
-    <row r="16" ht="14" customHeight="1">
-      <c r="A16" t="s" s="35">
+      <c r="I15" s="23"/>
+    </row>
+    <row r="16" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="36"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="13"/>
-      <c r="D16" t="s" s="16">
+      <c r="D16" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E16" t="s" s="16">
+      <c r="E16" s="16" t="s">
         <v>47</v>
       </c>
       <c r="F16" s="9"/>
-      <c r="G16" t="s" s="23">
+      <c r="G16" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H16" t="s" s="35">
+      <c r="H16" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="I16" s="24"/>
-    </row>
-    <row r="17" ht="14" customHeight="1">
-      <c r="A17" t="s" s="35">
+      <c r="I16" s="23"/>
+    </row>
+    <row r="17" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="B17" t="s" s="35">
+      <c r="B17" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="9"/>
-      <c r="E17" t="s" s="37">
+      <c r="C17" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="36" t="s">
         <v>45</v>
       </c>
       <c r="F17" s="9"/>
-      <c r="G17" t="s" s="23">
+      <c r="G17" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H17" t="s" s="35">
+      <c r="H17" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="I17" s="24"/>
-    </row>
-    <row r="18" ht="14" customHeight="1">
-      <c r="A18" t="s" s="35">
+      <c r="I17" s="23"/>
+    </row>
+    <row r="18" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="B18" t="s" s="11">
+      <c r="B18" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="9"/>
-      <c r="E18" t="s" s="37">
+      <c r="C18" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" s="36" t="s">
         <v>45</v>
       </c>
       <c r="F18" s="9"/>
-      <c r="G18" t="s" s="23">
+      <c r="G18" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H18" t="s" s="35">
+      <c r="H18" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="I18" s="24"/>
-    </row>
-    <row r="19" ht="14" customHeight="1">
-      <c r="A19" t="s" s="35">
+      <c r="I18" s="23"/>
+    </row>
+    <row r="19" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="36"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="13"/>
-      <c r="D19" t="s" s="16">
+      <c r="D19" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E19" t="s" s="38">
+      <c r="E19" s="37" t="s">
         <v>53</v>
       </c>
       <c r="F19" s="9"/>
-      <c r="G19" t="s" s="23">
+      <c r="G19" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H19" t="s" s="35">
+      <c r="H19" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="I19" s="24"/>
-    </row>
-    <row r="20" ht="14" customHeight="1">
-      <c r="A20" t="s" s="35">
+      <c r="I19" s="23"/>
+    </row>
+    <row r="20" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B20" t="s" s="35">
+      <c r="B20" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="9"/>
-      <c r="E20" t="s" s="37">
+      <c r="C20" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20" s="36" t="s">
         <v>45</v>
       </c>
       <c r="F20" s="9"/>
-      <c r="G20" t="s" s="23">
+      <c r="G20" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H20" t="s" s="35">
+      <c r="H20" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="I20" s="24"/>
-    </row>
-    <row r="21" ht="14" customHeight="1">
-      <c r="A21" t="s" s="35">
+      <c r="I20" s="23"/>
+    </row>
+    <row r="21" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="B21" t="s" s="35">
+      <c r="B21" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="9"/>
-      <c r="E21" t="s" s="37">
+      <c r="C21" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" s="36" t="s">
         <v>45</v>
       </c>
       <c r="F21" s="9"/>
-      <c r="G21" t="s" s="23">
+      <c r="G21" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H21" t="s" s="35">
+      <c r="H21" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="I21" s="24"/>
-    </row>
-    <row r="22" ht="13.55" customHeight="1">
-      <c r="A22" t="s" s="39">
+      <c r="I21" s="23"/>
+    </row>
+    <row r="22" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="26"/>
+      <c r="B22" s="25"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="27"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="26"/>
       <c r="I22" s="14"/>
     </row>
-    <row r="23" ht="14" customHeight="1">
-      <c r="A23" t="s" s="41">
+    <row r="23" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="42"/>
-      <c r="C23" t="s" s="43">
+      <c r="B23" s="41"/>
+      <c r="C23" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D23" t="s" s="44">
+      <c r="D23" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="E23" t="s" s="44">
+      <c r="E23" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="F23" s="45"/>
-      <c r="G23" t="s" s="46">
+      <c r="F23" s="44"/>
+      <c r="G23" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="H23" t="s" s="41">
+      <c r="H23" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="I23" s="47"/>
-    </row>
-    <row r="24" ht="14" customHeight="1">
-      <c r="A24" t="s" s="46">
+      <c r="I23" s="46"/>
+    </row>
+    <row r="24" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="42"/>
-      <c r="C24" t="s" s="43">
+      <c r="B24" s="41"/>
+      <c r="C24" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="D24" t="s" s="44">
+      <c r="D24" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="E24" t="s" s="44">
+      <c r="E24" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="F24" s="45"/>
-      <c r="G24" t="s" s="46">
+      <c r="F24" s="44"/>
+      <c r="G24" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="H24" t="s" s="48">
+      <c r="H24" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="I24" s="49"/>
-    </row>
-    <row r="25" ht="14" customHeight="1">
-      <c r="A25" t="s" s="35">
+      <c r="I24" s="48"/>
+    </row>
+    <row r="25" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="36"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="13"/>
       <c r="D25" s="9"/>
-      <c r="E25" t="s" s="16">
+      <c r="E25" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F25" s="50"/>
-      <c r="G25" t="s" s="11">
+      <c r="F25" s="49"/>
+      <c r="G25" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="H25" t="s" s="35">
+      <c r="H25" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="I25" s="24"/>
-    </row>
-    <row r="26" ht="30.75" customHeight="1">
-      <c r="A26" t="s" s="35">
+      <c r="I25" s="23"/>
+    </row>
+    <row r="26" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="36"/>
+      <c r="B26" s="35"/>
       <c r="C26" s="13"/>
-      <c r="D26" t="s" s="19">
+      <c r="D26" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="E26" t="s" s="16">
+      <c r="E26" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F26" t="s" s="51">
+      <c r="F26" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="G26" t="s" s="11">
+      <c r="G26" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="H26" t="s" s="35">
+      <c r="H26" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="I26" s="24"/>
-    </row>
-    <row r="27" ht="14" customHeight="1">
-      <c r="A27" t="s" s="35">
+      <c r="I26" s="23"/>
+    </row>
+    <row r="27" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B27" t="s" s="35">
+      <c r="B27" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="9"/>
-      <c r="E27" t="s" s="37">
+      <c r="C27" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="50"/>
-      <c r="G27" t="s" s="11">
+      <c r="F27" s="49"/>
+      <c r="G27" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="H27" t="s" s="35">
+      <c r="H27" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="I27" s="24"/>
-    </row>
-    <row r="28" ht="14" customHeight="1">
-      <c r="A28" t="s" s="35">
+      <c r="I27" s="23"/>
+    </row>
+    <row r="28" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="36"/>
+      <c r="B28" s="35"/>
       <c r="C28" s="13"/>
-      <c r="D28" t="s" s="16">
+      <c r="D28" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E28" t="s" s="16">
+      <c r="E28" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="F28" s="50"/>
-      <c r="G28" t="s" s="11">
+      <c r="F28" s="49"/>
+      <c r="G28" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="H28" t="s" s="35">
+      <c r="H28" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="I28" s="24"/>
-    </row>
-    <row r="29" ht="14" customHeight="1">
-      <c r="A29" t="s" s="35">
+      <c r="I28" s="23"/>
+    </row>
+    <row r="29" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="36"/>
+      <c r="B29" s="35"/>
       <c r="C29" s="13"/>
-      <c r="D29" t="s" s="16">
+      <c r="D29" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E29" t="s" s="16">
+      <c r="E29" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="50"/>
-      <c r="G29" t="s" s="11">
+      <c r="F29" s="49"/>
+      <c r="G29" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="H29" t="s" s="35">
+      <c r="H29" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="I29" s="24"/>
-    </row>
-    <row r="30" ht="14" customHeight="1">
-      <c r="A30" t="s" s="35">
+      <c r="I29" s="23"/>
+    </row>
+    <row r="30" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="36"/>
+      <c r="B30" s="35"/>
       <c r="C30" s="13"/>
-      <c r="D30" t="s" s="16">
+      <c r="D30" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E30" t="s" s="16">
+      <c r="E30" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="F30" s="50"/>
-      <c r="G30" t="s" s="11">
+      <c r="F30" s="49"/>
+      <c r="G30" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="H30" t="s" s="35">
+      <c r="H30" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="I30" s="24"/>
-    </row>
-    <row r="31" ht="13.55" customHeight="1">
-      <c r="A31" s="52"/>
-      <c r="B31" s="22"/>
+      <c r="I30" s="23"/>
+    </row>
+    <row r="31" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="51"/>
+      <c r="B31" s="21"/>
       <c r="C31" s="13"/>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
       <c r="I31" s="14"/>
     </row>
-    <row r="32" ht="39.55" customHeight="1">
-      <c r="A32" t="s" s="53">
+    <row r="32" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="54"/>
-      <c r="C32" t="s" s="55">
+      <c r="B32" s="53"/>
+      <c r="C32" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="D32" t="s" s="56">
+      <c r="D32" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="E32" t="s" s="57">
+      <c r="E32" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="F32" s="58"/>
-      <c r="G32" t="s" s="53">
+      <c r="F32" s="57"/>
+      <c r="G32" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="H32" t="s" s="59">
+      <c r="H32" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="I32" s="60"/>
-    </row>
-    <row r="33" ht="14" customHeight="1">
-      <c r="A33" t="s" s="35">
+      <c r="I32" s="59"/>
+    </row>
+    <row r="33" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="61"/>
-      <c r="E33" t="s" s="37">
+      <c r="B33" s="21"/>
+      <c r="C33" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="60" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F33" s="50"/>
-      <c r="G33" t="s" s="11">
+      <c r="F33" s="49"/>
+      <c r="G33" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="H33" t="s" s="35">
+      <c r="H33" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="I33" s="24"/>
-    </row>
-    <row r="34" ht="14" customHeight="1">
-      <c r="A34" t="s" s="35">
+      <c r="I33" s="23"/>
+    </row>
+    <row r="34" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="B34" t="s" s="35">
+      <c r="B34" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="9"/>
-      <c r="E34" t="s" s="37">
+      <c r="C34" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E34" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F34" s="50"/>
-      <c r="G34" t="s" s="11">
+      <c r="F34" s="49"/>
+      <c r="G34" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="H34" t="s" s="35">
+      <c r="H34" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="I34" s="24"/>
-    </row>
-    <row r="35" ht="14" customHeight="1">
-      <c r="A35" t="s" s="35">
+      <c r="I34" s="23"/>
+    </row>
+    <row r="35" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B35" t="s" s="62">
+      <c r="B35" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="9"/>
-      <c r="E35" t="s" s="37">
+      <c r="C35" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E35" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F35" s="50"/>
-      <c r="G35" t="s" s="11">
+      <c r="F35" s="49"/>
+      <c r="G35" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="H35" t="s" s="35">
+      <c r="H35" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="I35" s="24"/>
-    </row>
-    <row r="36" ht="37.5" customHeight="1">
-      <c r="A36" t="s" s="35">
+      <c r="I35" s="23"/>
+    </row>
+    <row r="36" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="52"/>
+      <c r="B36" s="51"/>
       <c r="C36" s="13"/>
-      <c r="D36" t="s" s="63">
+      <c r="D36" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="E36" t="s" s="19">
+      <c r="E36" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F36" s="50"/>
-      <c r="G36" t="s" s="11">
+      <c r="F36" s="49"/>
+      <c r="G36" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="H36" t="s" s="35">
+      <c r="H36" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="I36" s="24"/>
-    </row>
-    <row r="37" ht="37.5" customHeight="1">
-      <c r="A37" t="s" s="35">
+      <c r="I36" s="23"/>
+    </row>
+    <row r="37" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="52"/>
+      <c r="B37" s="51"/>
       <c r="C37" s="13"/>
-      <c r="D37" t="s" s="16">
+      <c r="D37" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="E37" t="s" s="16">
+      <c r="E37" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="F37" s="50"/>
-      <c r="G37" t="s" s="11">
+      <c r="F37" s="49"/>
+      <c r="G37" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="H37" t="s" s="35">
+      <c r="H37" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="I37" s="24"/>
-    </row>
-    <row r="38" ht="37.5" customHeight="1">
-      <c r="A38" t="s" s="64">
+      <c r="I37" s="23"/>
+    </row>
+    <row r="38" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="65"/>
+      <c r="B38" s="64"/>
       <c r="C38" s="13"/>
-      <c r="D38" t="s" s="16">
+      <c r="D38" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="E38" t="s" s="16">
+      <c r="E38" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="F38" s="50"/>
-      <c r="G38" t="s" s="66">
+      <c r="F38" s="49"/>
+      <c r="G38" s="65" t="s">
         <v>73</v>
       </c>
-      <c r="H38" t="s" s="64">
+      <c r="H38" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="I38" s="24"/>
-    </row>
-    <row r="39" ht="37.5" customHeight="1">
-      <c r="A39" t="s" s="67">
+      <c r="I38" s="23"/>
+    </row>
+    <row r="39" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="B39" t="s" s="15">
+      <c r="B39" s="15" t="s">
         <v>80</v>
       </c>
       <c r="C39" s="9"/>
-      <c r="D39" t="s" s="16">
+      <c r="D39" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="E39" t="s" s="16">
+      <c r="E39" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F39" s="50"/>
-      <c r="G39" t="s" s="68">
+      <c r="F39" s="49"/>
+      <c r="G39" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="H39" t="s" s="69">
+      <c r="H39" s="68" t="s">
         <v>79</v>
       </c>
       <c r="I39" s="13"/>
     </row>
-    <row r="40" ht="37.5" customHeight="1">
-      <c r="A40" t="s" s="70">
+    <row r="40" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="B40" t="s" s="15">
+      <c r="B40" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" t="s" s="37">
+      <c r="C40" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E40" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F40" s="50"/>
-      <c r="G40" t="s" s="11">
+      <c r="F40" s="49"/>
+      <c r="G40" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="H40" t="s" s="71">
+      <c r="H40" s="70" t="s">
         <v>81</v>
       </c>
       <c r="I40" s="13"/>
     </row>
-    <row r="41" ht="37.5" customHeight="1">
-      <c r="A41" t="s" s="72">
+    <row r="41" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="71" t="s">
         <v>82</v>
       </c>
-      <c r="B41" t="s" s="15">
+      <c r="B41" s="15" t="s">
         <v>80</v>
       </c>
       <c r="C41" s="9"/>
-      <c r="D41" t="s" s="63">
+      <c r="D41" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="E41" t="s" s="19">
+      <c r="E41" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F41" t="s" s="73">
+      <c r="F41" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="G41" t="s" s="66">
+      <c r="G41" s="65" t="s">
         <v>73</v>
       </c>
-      <c r="H41" t="s" s="74">
+      <c r="H41" s="73" t="s">
         <v>82</v>
       </c>
       <c r="I41" s="13"/>
     </row>
-    <row r="42" ht="13.55" customHeight="1">
-      <c r="A42" t="s" s="75">
+    <row r="42" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="76"/>
+      <c r="B42" s="75"/>
       <c r="C42" s="13"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="40"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="39"/>
       <c r="I42" s="14"/>
     </row>
-    <row r="43" ht="14" customHeight="1">
-      <c r="A43" t="s" s="35">
+    <row r="43" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="B43" s="52"/>
-      <c r="C43" t="s" s="15">
+      <c r="B43" s="51"/>
+      <c r="C43" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D43" t="s" s="16">
+      <c r="D43" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E43" t="s" s="16">
+      <c r="E43" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="F43" s="50"/>
-      <c r="G43" t="s" s="11">
+      <c r="F43" s="49"/>
+      <c r="G43" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H43" t="s" s="35">
+      <c r="H43" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="I43" s="24"/>
-    </row>
-    <row r="44" ht="91.5" customHeight="1">
-      <c r="A44" t="s" s="35">
+      <c r="I43" s="23"/>
+    </row>
+    <row r="44" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="B44" t="s" s="35">
+      <c r="B44" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="9"/>
-      <c r="E44" t="s" s="37">
+      <c r="C44" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E44" s="93" t="s">
+        <v>117</v>
+      </c>
+      <c r="F44" s="49"/>
+      <c r="G44" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H44" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="I44" s="23"/>
+    </row>
+    <row r="45" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E45" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F44" s="50"/>
-      <c r="G44" t="s" s="11">
+      <c r="F45" s="49"/>
+      <c r="G45" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H44" t="s" s="35">
-        <v>86</v>
-      </c>
-      <c r="I44" s="24"/>
-    </row>
-    <row r="45" ht="14" customHeight="1">
-      <c r="A45" t="s" s="35">
+      <c r="H45" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="B45" t="s" s="35">
-        <v>89</v>
-      </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="9"/>
-      <c r="E45" t="s" s="37">
+      <c r="I45" s="23"/>
+    </row>
+    <row r="46" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E46" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F45" s="50"/>
-      <c r="G45" t="s" s="11">
+      <c r="F46" s="49"/>
+      <c r="G46" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H45" t="s" s="35">
-        <v>88</v>
-      </c>
-      <c r="I45" s="24"/>
-    </row>
-    <row r="46" ht="14" customHeight="1">
-      <c r="A46" t="s" s="35">
+      <c r="H46" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="B46" t="s" s="35">
-        <v>91</v>
-      </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="9"/>
-      <c r="E46" t="s" s="37">
+      <c r="I46" s="23"/>
+    </row>
+    <row r="47" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E47" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F46" s="50"/>
-      <c r="G46" t="s" s="11">
+      <c r="F47" s="49"/>
+      <c r="G47" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H46" t="s" s="35">
-        <v>90</v>
-      </c>
-      <c r="I46" s="24"/>
-    </row>
-    <row r="47" ht="14" customHeight="1">
-      <c r="A47" t="s" s="35">
+      <c r="H47" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="B47" t="s" s="35">
-        <v>93</v>
-      </c>
-      <c r="C47" s="13"/>
-      <c r="D47" s="9"/>
-      <c r="E47" t="s" s="37">
+      <c r="I47" s="23"/>
+    </row>
+    <row r="48" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E48" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F47" s="50"/>
-      <c r="G47" t="s" s="11">
+      <c r="F48" s="49"/>
+      <c r="G48" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H47" t="s" s="35">
-        <v>92</v>
-      </c>
-      <c r="I47" s="24"/>
-    </row>
-    <row r="48" ht="14" customHeight="1">
-      <c r="A48" t="s" s="35">
+      <c r="H48" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="B48" t="s" s="35">
-        <v>95</v>
-      </c>
-      <c r="C48" s="13"/>
-      <c r="D48" s="9"/>
-      <c r="E48" t="s" s="37">
-        <v>45</v>
-      </c>
-      <c r="F48" s="50"/>
-      <c r="G48" t="s" s="11">
-        <v>85</v>
-      </c>
-      <c r="H48" t="s" s="35">
-        <v>94</v>
-      </c>
-      <c r="I48" s="24"/>
-    </row>
-    <row r="49" ht="14" customHeight="1">
-      <c r="A49" t="s" s="6">
+      <c r="I48" s="23"/>
+    </row>
+    <row r="49" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B49" s="52"/>
+      <c r="B49" s="51"/>
       <c r="C49" s="13"/>
       <c r="D49" s="9"/>
-      <c r="E49" t="s" s="37">
+      <c r="E49" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F49" s="40"/>
-      <c r="G49" s="27"/>
-      <c r="H49" s="27"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
       <c r="I49" s="14"/>
     </row>
-    <row r="50" ht="30.75" customHeight="1">
-      <c r="A50" t="s" s="35">
+    <row r="50" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="B50" s="52"/>
-      <c r="C50" t="s" s="15">
+      <c r="B50" s="51"/>
+      <c r="C50" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D50" t="s" s="16">
+      <c r="D50" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E50" t="s" s="77">
+      <c r="E50" s="76" t="s">
         <v>60</v>
       </c>
       <c r="F50" s="11"/>
-      <c r="G50" t="s" s="62">
+      <c r="G50" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="H50" t="s" s="78">
+      <c r="H50" s="77" t="s">
         <v>97</v>
       </c>
-      <c r="I50" s="24"/>
-    </row>
-    <row r="51" ht="30.75" customHeight="1">
-      <c r="A51" t="s" s="35">
+      <c r="I50" s="23"/>
+    </row>
+    <row r="51" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="36"/>
-      <c r="C51" t="s" s="15">
+      <c r="B51" s="35"/>
+      <c r="C51" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D51" t="s" s="16">
+      <c r="D51" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E51" t="s" s="79">
+      <c r="E51" s="78" t="s">
         <v>99</v>
       </c>
-      <c r="F51" t="s" s="80">
+      <c r="F51" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="G51" t="s" s="62">
+      <c r="G51" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="H51" t="s" s="35">
+      <c r="H51" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="I51" s="24"/>
-    </row>
-    <row r="52" ht="30.75" customHeight="1">
-      <c r="A52" t="s" s="35">
+      <c r="I51" s="23"/>
+    </row>
+    <row r="52" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="B52" s="36"/>
-      <c r="C52" t="s" s="81">
+      <c r="B52" s="35"/>
+      <c r="C52" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="D52" t="s" s="82">
+      <c r="D52" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="E52" t="s" s="83">
+      <c r="E52" s="82" t="s">
         <v>102</v>
       </c>
-      <c r="F52" s="84"/>
-      <c r="G52" t="s" s="62">
+      <c r="F52" s="83"/>
+      <c r="G52" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="H52" t="s" s="35">
+      <c r="H52" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="I52" s="85"/>
+      <c r="I52" s="84"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I30" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -3301,56 +3350,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.1719" style="86" customWidth="1"/>
-    <col min="2" max="2" width="42.3516" style="86" customWidth="1"/>
-    <col min="3" max="3" width="13.6719" style="86" customWidth="1"/>
-    <col min="4" max="4" width="23.3516" style="86" customWidth="1"/>
-    <col min="5" max="5" width="28" style="86" customWidth="1"/>
-    <col min="6" max="6" width="31.3516" style="86" customWidth="1"/>
-    <col min="7" max="7" width="26.3516" style="86" customWidth="1"/>
-    <col min="8" max="8" width="16.5" style="86" customWidth="1"/>
-    <col min="9" max="9" width="27.5" style="86" customWidth="1"/>
-    <col min="10" max="10" width="13.6719" style="86" customWidth="1"/>
-    <col min="11" max="16384" width="8.85156" style="86" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28" style="1" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" t="s" s="2">
+      <c r="B1" s="85"/>
+      <c r="C1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="87"/>
-      <c r="H1" t="s" s="88">
+      <c r="G1" s="85"/>
+      <c r="H1" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s" s="89">
+      <c r="I1" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s" s="88">
+      <c r="J1" s="86" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="6">
+    <row r="2" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="7"/>
@@ -3363,8 +3413,8 @@
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="90">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="88" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="12"/>
@@ -3377,1005 +3427,1005 @@
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="11">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="12"/>
-      <c r="C4" t="s" s="15">
+      <c r="C4" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="D4" t="s" s="19">
+      <c r="D4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s" s="16">
+      <c r="E4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s" s="16">
+      <c r="F4" s="16" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="9"/>
-      <c r="H4" t="s" s="19">
+      <c r="H4" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="I4" t="s" s="20">
+      <c r="I4" s="19" t="s">
         <v>16</v>
       </c>
       <c r="J4" s="9"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="11">
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" t="s" s="15">
+      <c r="C5" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="D5" t="s" s="19">
+      <c r="D5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s" s="16">
+      <c r="E5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s" s="19">
+      <c r="F5" s="18" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" t="s" s="19">
+      <c r="H5" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="I5" t="s" s="20">
+      <c r="I5" s="19" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="9"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="11">
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" t="s" s="15">
+      <c r="C6" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="D6" t="s" s="19">
+      <c r="D6" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s" s="16">
+      <c r="E6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F6" t="s" s="16">
+      <c r="F6" s="16" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" t="s" s="19">
+      <c r="H6" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="I6" t="s" s="20">
+      <c r="I6" s="19" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="9"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="11">
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="12"/>
-      <c r="C7" t="s" s="15">
+      <c r="C7" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="D7" t="s" s="19">
+      <c r="D7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E7" t="s" s="16">
+      <c r="E7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F7" t="s" s="19">
+      <c r="F7" s="18" t="s">
         <v>24</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" t="s" s="19">
+      <c r="H7" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="I7" t="s" s="20">
+      <c r="I7" s="19" t="s">
         <v>25</v>
       </c>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="11">
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="12"/>
-      <c r="C8" t="s" s="15">
+      <c r="C8" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="D8" t="s" s="19">
+      <c r="D8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E8" t="s" s="16">
+      <c r="E8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F8" t="s" s="16">
+      <c r="F8" s="16" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="9"/>
-      <c r="H8" t="s" s="19">
+      <c r="H8" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="I8" t="s" s="21">
+      <c r="I8" s="20" t="s">
         <v>28</v>
       </c>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" ht="14" customHeight="1">
-      <c r="A9" t="s" s="11">
+    <row r="9" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" t="s" s="15">
+      <c r="B9" s="21"/>
+      <c r="C9" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="D9" t="s" s="19">
+      <c r="D9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E9" t="s" s="16">
+      <c r="E9" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="F9" t="s" s="16">
+      <c r="F9" s="16" t="s">
         <v>30</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" t="s" s="23">
+      <c r="H9" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="I9" t="s" s="11">
+      <c r="I9" s="11" t="s">
         <v>29</v>
       </c>
       <c r="J9" s="13"/>
     </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" t="s" s="25">
+    <row r="10" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="26"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
-      <c r="I10" s="27"/>
+      <c r="I10" s="26"/>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" ht="14" customHeight="1">
-      <c r="A11" t="s" s="35">
+    <row r="11" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" t="s" s="15">
+      <c r="B11" s="35"/>
+      <c r="C11" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D11" t="s" s="19">
+      <c r="D11" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E11" t="s" s="16">
+      <c r="E11" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F11" t="s" s="16">
+      <c r="F11" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="G11" t="s" s="19">
+      <c r="G11" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="H11" t="s" s="23">
+      <c r="H11" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="I11" t="s" s="35">
+      <c r="I11" s="34" t="s">
         <v>38</v>
       </c>
       <c r="J11" s="13"/>
     </row>
-    <row r="12" ht="14" customHeight="1">
-      <c r="A12" t="s" s="35">
+    <row r="12" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="36"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="13"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
-      <c r="F12" t="s" s="16">
+      <c r="F12" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="G12" t="s" s="19">
+      <c r="G12" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H12" t="s" s="23">
+      <c r="H12" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="I12" t="s" s="35">
+      <c r="I12" s="34" t="s">
         <v>41</v>
       </c>
       <c r="J12" s="13"/>
     </row>
-    <row r="13" ht="14" customHeight="1">
-      <c r="A13" t="s" s="35">
+    <row r="13" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B13" t="s" s="35">
+      <c r="B13" s="34" t="s">
         <v>44</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
-      <c r="F13" t="s" s="91">
+      <c r="F13" s="89" t="s">
         <v>45</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" t="s" s="23">
+      <c r="H13" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="I13" t="s" s="35">
+      <c r="I13" s="34" t="s">
         <v>43</v>
       </c>
       <c r="J13" s="13"/>
     </row>
-    <row r="14" ht="14" customHeight="1">
-      <c r="A14" t="s" s="35">
+    <row r="14" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="36"/>
-      <c r="C14" t="s" s="15">
+      <c r="B14" s="35"/>
+      <c r="C14" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D14" t="s" s="19">
+      <c r="D14" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E14" t="s" s="16">
+      <c r="E14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F14" t="s" s="16">
+      <c r="F14" s="16" t="s">
         <v>47</v>
       </c>
       <c r="G14" s="9"/>
-      <c r="H14" t="s" s="23">
+      <c r="H14" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="I14" t="s" s="35">
+      <c r="I14" s="34" t="s">
         <v>46</v>
       </c>
       <c r="J14" s="13"/>
     </row>
-    <row r="15" ht="14" customHeight="1">
-      <c r="A15" t="s" s="35">
+    <row r="15" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="B15" t="s" s="35">
+      <c r="B15" s="34" t="s">
         <v>49</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
-      <c r="F15" t="s" s="91">
+      <c r="F15" s="89" t="s">
         <v>45</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" t="s" s="23">
+      <c r="H15" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="I15" t="s" s="35">
+      <c r="I15" s="34" t="s">
         <v>48</v>
       </c>
       <c r="J15" s="13"/>
     </row>
-    <row r="16" ht="14" customHeight="1">
-      <c r="A16" t="s" s="35">
+    <row r="16" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="B16" t="s" s="11">
+      <c r="B16" s="11" t="s">
         <v>51</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
-      <c r="F16" t="s" s="91">
+      <c r="F16" s="89" t="s">
         <v>45</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" t="s" s="23">
+      <c r="H16" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="I16" t="s" s="35">
+      <c r="I16" s="34" t="s">
         <v>50</v>
       </c>
       <c r="J16" s="13"/>
     </row>
-    <row r="17" ht="14" customHeight="1">
-      <c r="A17" t="s" s="35">
+    <row r="17" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" t="s" s="15">
+      <c r="B17" s="35"/>
+      <c r="C17" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D17" t="s" s="19">
+      <c r="D17" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E17" t="s" s="16">
+      <c r="E17" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F17" t="s" s="92">
+      <c r="F17" s="90" t="s">
         <v>53</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" t="s" s="23">
+      <c r="H17" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="I17" t="s" s="35">
+      <c r="I17" s="34" t="s">
         <v>52</v>
       </c>
       <c r="J17" s="13"/>
     </row>
-    <row r="18" ht="14" customHeight="1">
-      <c r="A18" t="s" s="35">
+    <row r="18" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B18" t="s" s="35">
+      <c r="B18" s="34" t="s">
         <v>55</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
-      <c r="F18" t="s" s="91">
+      <c r="F18" s="89" t="s">
         <v>45</v>
       </c>
       <c r="G18" s="9"/>
-      <c r="H18" t="s" s="23">
+      <c r="H18" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="I18" t="s" s="35">
+      <c r="I18" s="34" t="s">
         <v>54</v>
       </c>
       <c r="J18" s="13"/>
     </row>
-    <row r="19" ht="14" customHeight="1">
-      <c r="A19" t="s" s="35">
+    <row r="19" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="B19" t="s" s="35">
+      <c r="B19" s="34" t="s">
         <v>57</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
-      <c r="F19" t="s" s="91">
+      <c r="F19" s="89" t="s">
         <v>45</v>
       </c>
       <c r="G19" s="9"/>
-      <c r="H19" t="s" s="23">
+      <c r="H19" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="I19" t="s" s="35">
+      <c r="I19" s="34" t="s">
         <v>56</v>
       </c>
       <c r="J19" s="13"/>
     </row>
-    <row r="20" ht="13.55" customHeight="1">
-      <c r="A20" t="s" s="39">
+    <row r="20" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="26"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="27"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="26"/>
       <c r="J20" s="9"/>
     </row>
-    <row r="21" ht="14" customHeight="1">
-      <c r="A21" t="s" s="35">
+    <row r="21" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="52"/>
-      <c r="C21" t="s" s="15">
+      <c r="B21" s="51"/>
+      <c r="C21" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="D21" t="s" s="19">
+      <c r="D21" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E21" t="s" s="16">
+      <c r="E21" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F21" t="s" s="16">
+      <c r="F21" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="G21" s="50"/>
-      <c r="H21" t="s" s="90">
+      <c r="G21" s="49"/>
+      <c r="H21" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="I21" t="s" s="35">
+      <c r="I21" s="34" t="s">
         <v>59</v>
       </c>
       <c r="J21" s="13"/>
     </row>
-    <row r="22" ht="13.55" customHeight="1">
-      <c r="A22" t="s" s="90">
+    <row r="22" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="52"/>
+      <c r="B22" s="51"/>
       <c r="C22" s="13"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
       <c r="J22" s="9"/>
     </row>
-    <row r="23" ht="14" customHeight="1">
-      <c r="A23" t="s" s="35">
+    <row r="23" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="36"/>
-      <c r="C23" t="s" s="15">
+      <c r="B23" s="35"/>
+      <c r="C23" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D23" t="s" s="19">
+      <c r="D23" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E23" t="s" s="16">
+      <c r="E23" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F23" t="s" s="16">
+      <c r="F23" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="50"/>
-      <c r="H23" t="s" s="90">
+      <c r="G23" s="49"/>
+      <c r="H23" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="I23" t="s" s="35">
+      <c r="I23" s="34" t="s">
         <v>64</v>
       </c>
       <c r="J23" s="13"/>
     </row>
-    <row r="24" ht="30.75" customHeight="1">
-      <c r="A24" t="s" s="35">
+    <row r="24" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="36"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="13"/>
       <c r="D24" s="9"/>
-      <c r="E24" t="s" s="19">
+      <c r="E24" s="18" t="s">
         <v>67</v>
       </c>
       <c r="F24" s="9"/>
-      <c r="G24" t="s" s="51">
+      <c r="G24" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="H24" t="s" s="90">
+      <c r="H24" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="I24" t="s" s="35">
+      <c r="I24" s="34" t="s">
         <v>66</v>
       </c>
       <c r="J24" s="13"/>
     </row>
-    <row r="25" ht="14" customHeight="1">
-      <c r="A25" t="s" s="35">
+    <row r="25" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B25" t="s" s="35">
+      <c r="B25" s="34" t="s">
         <v>44</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
-      <c r="F25" t="s" s="91">
+      <c r="F25" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="G25" s="50"/>
-      <c r="H25" t="s" s="90">
+      <c r="G25" s="49"/>
+      <c r="H25" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="I25" t="s" s="35">
+      <c r="I25" s="34" t="s">
         <v>43</v>
       </c>
       <c r="J25" s="13"/>
     </row>
-    <row r="26" ht="14" customHeight="1">
-      <c r="A26" t="s" s="35">
+    <row r="26" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" t="s" s="15">
+      <c r="B26" s="35"/>
+      <c r="C26" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D26" t="s" s="19">
+      <c r="D26" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E26" t="s" s="16">
+      <c r="E26" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F26" t="s" s="16">
+      <c r="F26" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="G26" s="50"/>
-      <c r="H26" t="s" s="90">
+      <c r="G26" s="49"/>
+      <c r="H26" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="I26" t="s" s="35">
+      <c r="I26" s="34" t="s">
         <v>46</v>
       </c>
       <c r="J26" s="13"/>
     </row>
-    <row r="27" ht="14" customHeight="1">
-      <c r="A27" t="s" s="35">
+    <row r="27" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" t="s" s="15">
+      <c r="B27" s="35"/>
+      <c r="C27" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D27" t="s" s="19">
+      <c r="D27" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E27" t="s" s="16">
+      <c r="E27" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F27" t="s" s="16">
+      <c r="F27" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="G27" s="50"/>
-      <c r="H27" t="s" s="90">
+      <c r="G27" s="49"/>
+      <c r="H27" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="I27" t="s" s="35">
+      <c r="I27" s="34" t="s">
         <v>69</v>
       </c>
       <c r="J27" s="13"/>
     </row>
-    <row r="28" ht="14" customHeight="1">
-      <c r="A28" t="s" s="35">
+    <row r="28" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" t="s" s="15">
+      <c r="B28" s="35"/>
+      <c r="C28" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D28" t="s" s="19">
+      <c r="D28" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E28" t="s" s="16">
+      <c r="E28" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F28" t="s" s="16">
+      <c r="F28" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="G28" s="50"/>
-      <c r="H28" t="s" s="90">
+      <c r="G28" s="49"/>
+      <c r="H28" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="I28" t="s" s="35">
+      <c r="I28" s="34" t="s">
         <v>71</v>
       </c>
       <c r="J28" s="13"/>
     </row>
-    <row r="29" ht="13.55" customHeight="1">
-      <c r="A29" t="s" s="90">
+    <row r="29" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="22"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="13"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
       <c r="J29" s="9"/>
     </row>
-    <row r="30" ht="37.5" customHeight="1">
-      <c r="A30" t="s" s="35">
+    <row r="30" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="22"/>
-      <c r="C30" t="s" s="15">
+      <c r="B30" s="21"/>
+      <c r="C30" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D30" t="s" s="19">
+      <c r="D30" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E30" t="s" s="63">
+      <c r="E30" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="F30" t="s" s="16">
+      <c r="F30" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="G30" s="50"/>
-      <c r="H30" t="s" s="90">
+      <c r="G30" s="49"/>
+      <c r="H30" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="I30" t="s" s="35">
+      <c r="I30" s="34" t="s">
         <v>64</v>
       </c>
       <c r="J30" s="13"/>
     </row>
-    <row r="31" ht="13.55" customHeight="1">
-      <c r="A31" t="s" s="35">
+    <row r="31" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="B31" t="s" s="35">
+      <c r="B31" s="34" t="s">
         <v>77</v>
       </c>
       <c r="C31" s="13"/>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
-      <c r="G31" s="50"/>
-      <c r="H31" t="s" s="90">
+      <c r="G31" s="49"/>
+      <c r="H31" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="I31" t="s" s="35">
+      <c r="I31" s="34" t="s">
         <v>66</v>
       </c>
       <c r="J31" s="13"/>
     </row>
-    <row r="32" ht="14" customHeight="1">
-      <c r="A32" t="s" s="35">
+    <row r="32" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B32" t="s" s="62">
+      <c r="B32" s="61" t="s">
         <v>78</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
-      <c r="F32" t="s" s="91">
+      <c r="F32" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="G32" s="50"/>
-      <c r="H32" t="s" s="90">
+      <c r="G32" s="49"/>
+      <c r="H32" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="I32" t="s" s="35">
+      <c r="I32" s="34" t="s">
         <v>43</v>
       </c>
       <c r="J32" s="13"/>
     </row>
-    <row r="33" ht="37.5" customHeight="1">
-      <c r="A33" t="s" s="35">
+    <row r="33" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="52"/>
-      <c r="C33" t="s" s="15">
+      <c r="B33" s="51"/>
+      <c r="C33" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D33" t="s" s="19">
+      <c r="D33" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E33" t="s" s="63">
+      <c r="E33" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="F33" t="s" s="19">
+      <c r="F33" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="G33" s="50"/>
-      <c r="H33" t="s" s="90">
+      <c r="G33" s="49"/>
+      <c r="H33" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="I33" t="s" s="35">
+      <c r="I33" s="34" t="s">
         <v>46</v>
       </c>
       <c r="J33" s="13"/>
     </row>
-    <row r="34" ht="37.5" customHeight="1">
-      <c r="A34" t="s" s="35">
+    <row r="34" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="52"/>
-      <c r="C34" t="s" s="15">
+      <c r="B34" s="51"/>
+      <c r="C34" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D34" t="s" s="19">
+      <c r="D34" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E34" t="s" s="63">
+      <c r="E34" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="F34" t="s" s="16">
+      <c r="F34" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="G34" s="50"/>
-      <c r="H34" t="s" s="90">
+      <c r="G34" s="49"/>
+      <c r="H34" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="I34" t="s" s="35">
+      <c r="I34" s="34" t="s">
         <v>69</v>
       </c>
       <c r="J34" s="13"/>
     </row>
-    <row r="35" ht="37.5" customHeight="1">
-      <c r="A35" t="s" s="35">
+    <row r="35" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="22"/>
-      <c r="C35" t="s" s="15">
+      <c r="B35" s="21"/>
+      <c r="C35" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D35" t="s" s="19">
+      <c r="D35" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E35" t="s" s="63">
+      <c r="E35" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="F35" t="s" s="16">
+      <c r="F35" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="G35" s="50"/>
-      <c r="H35" t="s" s="90">
+      <c r="G35" s="49"/>
+      <c r="H35" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="I35" t="s" s="35">
+      <c r="I35" s="34" t="s">
         <v>71</v>
       </c>
       <c r="J35" s="13"/>
     </row>
-    <row r="36" ht="13.55" customHeight="1">
-      <c r="A36" t="s" s="6">
+    <row r="36" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B36" s="52"/>
+      <c r="B36" s="51"/>
       <c r="C36" s="13"/>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="27"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
       <c r="J36" s="9"/>
     </row>
-    <row r="37" ht="14" customHeight="1">
-      <c r="A37" t="s" s="35">
+    <row r="37" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="52"/>
-      <c r="C37" t="s" s="15">
+      <c r="B37" s="51"/>
+      <c r="C37" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="D37" t="s" s="19">
+      <c r="D37" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E37" t="s" s="16">
+      <c r="E37" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F37" t="s" s="16">
+      <c r="F37" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="G37" s="50"/>
-      <c r="H37" t="s" s="11">
+      <c r="G37" s="49"/>
+      <c r="H37" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="I37" t="s" s="35">
+      <c r="I37" s="34" t="s">
         <v>59</v>
       </c>
       <c r="J37" s="13"/>
     </row>
-    <row r="38" ht="91.5" customHeight="1">
-      <c r="A38" t="s" s="35">
+    <row r="38" spans="1:10" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="B38" t="s" s="35">
+      <c r="B38" s="34" t="s">
         <v>87</v>
       </c>
       <c r="C38" s="13"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
-      <c r="F38" t="s" s="91">
+      <c r="F38" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="G38" s="50"/>
-      <c r="H38" t="s" s="11">
+      <c r="G38" s="49"/>
+      <c r="H38" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="I38" t="s" s="35">
+      <c r="I38" s="34" t="s">
         <v>86</v>
       </c>
       <c r="J38" s="13"/>
     </row>
-    <row r="39" ht="14" customHeight="1">
-      <c r="A39" t="s" s="35">
+    <row r="39" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="B39" t="s" s="35">
+      <c r="B39" s="34" t="s">
         <v>89</v>
       </c>
       <c r="C39" s="13"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
-      <c r="F39" t="s" s="91">
+      <c r="F39" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="G39" s="50"/>
-      <c r="H39" t="s" s="11">
+      <c r="G39" s="49"/>
+      <c r="H39" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="I39" t="s" s="35">
+      <c r="I39" s="34" t="s">
         <v>88</v>
       </c>
       <c r="J39" s="13"/>
     </row>
-    <row r="40" ht="14" customHeight="1">
-      <c r="A40" t="s" s="35">
+    <row r="40" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="B40" t="s" s="35">
+      <c r="B40" s="34" t="s">
         <v>91</v>
       </c>
       <c r="C40" s="13"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
-      <c r="F40" t="s" s="91">
+      <c r="F40" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="G40" s="50"/>
-      <c r="H40" t="s" s="11">
+      <c r="G40" s="49"/>
+      <c r="H40" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="I40" t="s" s="35">
+      <c r="I40" s="34" t="s">
         <v>90</v>
       </c>
       <c r="J40" s="13"/>
     </row>
-    <row r="41" ht="14" customHeight="1">
-      <c r="A41" t="s" s="35">
+    <row r="41" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="B41" t="s" s="35">
+      <c r="B41" s="34" t="s">
         <v>93</v>
       </c>
       <c r="C41" s="13"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
-      <c r="F41" t="s" s="91">
+      <c r="F41" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="G41" s="50"/>
-      <c r="H41" t="s" s="11">
+      <c r="G41" s="49"/>
+      <c r="H41" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="I41" t="s" s="35">
+      <c r="I41" s="34" t="s">
         <v>92</v>
       </c>
       <c r="J41" s="13"/>
     </row>
-    <row r="42" ht="14" customHeight="1">
-      <c r="A42" t="s" s="35">
+    <row r="42" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="B42" t="s" s="35">
+      <c r="B42" s="34" t="s">
         <v>95</v>
       </c>
       <c r="C42" s="13"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
-      <c r="F42" t="s" s="91">
+      <c r="F42" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="G42" s="50"/>
-      <c r="H42" t="s" s="11">
+      <c r="G42" s="49"/>
+      <c r="H42" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="I42" t="s" s="35">
+      <c r="I42" s="34" t="s">
         <v>94</v>
       </c>
       <c r="J42" s="13"/>
     </row>
-    <row r="43" ht="14" customHeight="1">
-      <c r="A43" t="s" s="6">
+    <row r="43" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B43" s="52"/>
+      <c r="B43" s="51"/>
       <c r="C43" s="13"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
-      <c r="F43" t="s" s="91">
+      <c r="F43" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="G43" s="40"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
       <c r="J43" s="9"/>
     </row>
-    <row r="44" ht="30.75" customHeight="1">
-      <c r="A44" t="s" s="35">
+    <row r="44" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="B44" s="52"/>
-      <c r="C44" t="s" s="15">
+      <c r="B44" s="51"/>
+      <c r="C44" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="D44" t="s" s="19">
+      <c r="D44" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E44" t="s" s="16">
+      <c r="E44" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F44" t="s" s="77">
+      <c r="F44" s="76" t="s">
         <v>60</v>
       </c>
       <c r="G44" s="11"/>
-      <c r="H44" t="s" s="62">
+      <c r="H44" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="I44" t="s" s="78">
+      <c r="I44" s="77" t="s">
         <v>97</v>
       </c>
       <c r="J44" s="13"/>
     </row>
-    <row r="45" ht="30.75" customHeight="1">
-      <c r="A45" t="s" s="35">
+    <row r="45" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="B45" s="36"/>
-      <c r="C45" t="s" s="15">
+      <c r="B45" s="35"/>
+      <c r="C45" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="D45" t="s" s="19">
+      <c r="D45" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E45" t="s" s="16">
+      <c r="E45" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F45" t="s" s="93">
+      <c r="F45" s="91" t="s">
         <v>109</v>
       </c>
-      <c r="G45" s="94"/>
-      <c r="H45" t="s" s="62">
+      <c r="G45" s="92"/>
+      <c r="H45" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="I45" t="s" s="35">
+      <c r="I45" s="34" t="s">
         <v>98</v>
       </c>
       <c r="J45" s="13"/>
     </row>
-    <row r="46" ht="30.75" customHeight="1">
-      <c r="A46" t="s" s="35">
+    <row r="46" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="B46" s="36"/>
-      <c r="C46" t="s" s="15">
+      <c r="B46" s="35"/>
+      <c r="C46" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="D46" t="s" s="19">
+      <c r="D46" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E46" t="s" s="16">
+      <c r="E46" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F46" t="s" s="92">
+      <c r="F46" s="90" t="s">
         <v>102</v>
       </c>
-      <c r="G46" s="50"/>
-      <c r="H46" t="s" s="62">
+      <c r="G46" s="49"/>
+      <c r="H46" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="I46" t="s" s="35">
+      <c r="I46" s="34" t="s">
         <v>96</v>
       </c>
       <c r="J46" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" location="" tooltip="" display="Company"/>
-    <hyperlink ref="H5" r:id="rId2" location="" tooltip="" display="Company"/>
-    <hyperlink ref="H6" r:id="rId3" location="" tooltip="" display="Company"/>
-    <hyperlink ref="H7" r:id="rId4" location="" tooltip="" display="Company"/>
-    <hyperlink ref="H8" r:id="rId5" location="" tooltip="" display="Company"/>
-    <hyperlink ref="H9" r:id="rId6" location="" tooltip="" display="Company"/>
+    <hyperlink ref="H4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="H5" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="H6" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="H7" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="H8" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="H9" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>